<commit_message>
Remove obsolete FacoDMEK_Optimization_Results.xlsx file to streamline project resources
</commit_message>
<xml_diff>
--- a/FacoDMEK.xlsx
+++ b/FacoDMEK.xlsx
@@ -5,18 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\offic\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Websites\faco-dmek\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAB1A6D8-1765-4959-ACF9-36DBCBEBB57D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A48D2B0B-6E74-4600-B9C7-2544AA1D9D37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cleaned Data" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Cleaned Data'!$B$1:$AD$98</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Cleaned Data'!$B$1:$AC$98</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="115">
   <si>
     <t>IOL Power</t>
   </si>
@@ -351,9 +351,6 @@
   </si>
   <si>
     <t>Fuchs</t>
-  </si>
-  <si>
-    <t>FARE TORNARE</t>
   </si>
   <si>
     <t>Scompenso</t>
@@ -821,25 +818,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AD98"/>
+  <dimension ref="A1:AC98"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="AD12" sqref="AD12"/>
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="H1" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="Q99" sqref="Q99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="11.2109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="19.4375" customWidth="1"/>
-    <col min="3" max="8" width="10.25" customWidth="1"/>
-    <col min="9" max="10" width="14.875" customWidth="1"/>
-    <col min="11" max="18" width="10.25" customWidth="1"/>
-    <col min="19" max="19" width="13.6875" customWidth="1"/>
-    <col min="20" max="29" width="10.25" customWidth="1"/>
-    <col min="30" max="30" width="7.75" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="3" max="8" width="10.2109375" customWidth="1"/>
+    <col min="9" max="10" width="14.85546875" customWidth="1"/>
+    <col min="11" max="18" width="10.2109375" customWidth="1"/>
+    <col min="19" max="19" width="13.7109375" customWidth="1"/>
+    <col min="20" max="29" width="10.2109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="52.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:29" ht="52.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>87</v>
       </c>
@@ -868,7 +866,7 @@
         <v>95</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K1" s="5" t="s">
         <v>96</v>
@@ -901,35 +899,34 @@
         <v>1</v>
       </c>
       <c r="U1" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="V1" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="W1" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="W1" s="7" t="s">
-        <v>115</v>
-      </c>
       <c r="X1" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Y1" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Z1" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AA1" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AB1" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC1" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="AC1" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="AD1" s="8"/>
     </row>
-    <row r="2" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="9">
         <v>1</v>
       </c>
@@ -979,7 +976,10 @@
       <c r="P2" s="15">
         <v>4.0599999999999996</v>
       </c>
-      <c r="Q2" s="15"/>
+      <c r="Q2" s="15">
+        <f>T2</f>
+        <v>594</v>
+      </c>
       <c r="R2" s="15">
         <v>12</v>
       </c>
@@ -1019,9 +1019,8 @@
       <c r="AC2" s="15">
         <v>-6.2</v>
       </c>
-      <c r="AD2" s="15"/>
     </row>
-    <row r="3" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="9">
         <v>2</v>
       </c>
@@ -1113,9 +1112,8 @@
       <c r="AC3" s="15">
         <v>-6.4</v>
       </c>
-      <c r="AD3" s="15"/>
     </row>
-    <row r="4" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="9">
         <v>3</v>
       </c>
@@ -1205,9 +1203,8 @@
       <c r="AC4" s="15">
         <v>-6.3</v>
       </c>
-      <c r="AD4" s="15"/>
     </row>
-    <row r="5" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="9">
         <v>4</v>
       </c>
@@ -1299,9 +1296,8 @@
       <c r="AC5" s="15">
         <v>-5.5</v>
       </c>
-      <c r="AD5" s="15"/>
     </row>
-    <row r="6" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="9">
         <v>5</v>
       </c>
@@ -1393,9 +1389,8 @@
       <c r="AC6" s="15">
         <v>-5.7</v>
       </c>
-      <c r="AD6" s="15"/>
     </row>
-    <row r="7" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="9">
         <v>6</v>
       </c>
@@ -1487,9 +1482,8 @@
       <c r="AC7" s="15">
         <v>-5.7</v>
       </c>
-      <c r="AD7" s="15"/>
     </row>
-    <row r="8" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="9">
         <v>7</v>
       </c>
@@ -1581,9 +1575,8 @@
       <c r="AC8" s="15">
         <v>-5.8</v>
       </c>
-      <c r="AD8" s="15"/>
     </row>
-    <row r="9" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="9">
         <v>8</v>
       </c>
@@ -1675,9 +1668,8 @@
       <c r="AC9" s="15">
         <v>-5.7</v>
       </c>
-      <c r="AD9" s="15"/>
     </row>
-    <row r="10" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="9">
         <v>9</v>
       </c>
@@ -1769,9 +1761,8 @@
       <c r="AC10" s="15">
         <v>-5.6</v>
       </c>
-      <c r="AD10" s="15"/>
     </row>
-    <row r="11" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="9">
         <v>10</v>
       </c>
@@ -1863,9 +1854,8 @@
       <c r="AC11" s="15">
         <v>-5.9</v>
       </c>
-      <c r="AD11" s="15"/>
     </row>
-    <row r="12" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="9">
         <v>11</v>
       </c>
@@ -1957,9 +1947,8 @@
       <c r="AC12" s="15">
         <v>-5.5</v>
       </c>
-      <c r="AD12" s="15"/>
     </row>
-    <row r="13" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="9">
         <v>12</v>
       </c>
@@ -2049,9 +2038,8 @@
       <c r="AC13" s="15">
         <v>-4.5999999999999996</v>
       </c>
-      <c r="AD13" s="15"/>
     </row>
-    <row r="14" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="9">
         <v>13</v>
       </c>
@@ -2143,9 +2131,8 @@
       <c r="AC14" s="15">
         <v>-5.4</v>
       </c>
-      <c r="AD14" s="15"/>
     </row>
-    <row r="15" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="9">
         <v>14</v>
       </c>
@@ -2237,9 +2224,8 @@
       <c r="AC15" s="15">
         <v>-5.8</v>
       </c>
-      <c r="AD15" s="15"/>
     </row>
-    <row r="16" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="9">
         <v>15</v>
       </c>
@@ -2331,9 +2317,8 @@
       <c r="AC16" s="15">
         <v>-5.5</v>
       </c>
-      <c r="AD16" s="15"/>
     </row>
-    <row r="17" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="9">
         <v>16</v>
       </c>
@@ -2383,7 +2368,10 @@
       <c r="P17" s="15">
         <v>4.8099999999999996</v>
       </c>
-      <c r="Q17" s="15"/>
+      <c r="Q17" s="15">
+        <f>T17</f>
+        <v>638</v>
+      </c>
       <c r="R17" s="15">
         <v>22.5</v>
       </c>
@@ -2423,9 +2411,8 @@
       <c r="AC17" s="15">
         <v>-5.4</v>
       </c>
-      <c r="AD17" s="15"/>
     </row>
-    <row r="18" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="9">
         <v>17</v>
       </c>
@@ -2517,9 +2504,8 @@
       <c r="AC18" s="15">
         <v>-6.2</v>
       </c>
-      <c r="AD18" s="15"/>
     </row>
-    <row r="19" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="9">
         <v>18</v>
       </c>
@@ -2609,9 +2595,8 @@
       <c r="AC19" s="15">
         <v>-5.3</v>
       </c>
-      <c r="AD19" s="15"/>
     </row>
-    <row r="20" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="9">
         <v>19</v>
       </c>
@@ -2699,9 +2684,8 @@
       <c r="AC20" s="15">
         <v>-5.2</v>
       </c>
-      <c r="AD20" s="15"/>
     </row>
-    <row r="21" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="9">
         <v>20</v>
       </c>
@@ -2793,9 +2777,8 @@
       <c r="AC21" s="15">
         <v>-5</v>
       </c>
-      <c r="AD21" s="15"/>
     </row>
-    <row r="22" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="9">
         <v>21</v>
       </c>
@@ -2887,9 +2870,8 @@
       <c r="AC22" s="15">
         <v>-5.2</v>
       </c>
-      <c r="AD22" s="15"/>
     </row>
-    <row r="23" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="9">
         <v>22</v>
       </c>
@@ -2981,9 +2963,8 @@
       <c r="AC23" s="15">
         <v>-6</v>
       </c>
-      <c r="AD23" s="15"/>
     </row>
-    <row r="24" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="9">
         <v>23</v>
       </c>
@@ -3075,9 +3056,8 @@
       <c r="AC24" s="15">
         <v>-5.0999999999999996</v>
       </c>
-      <c r="AD24" s="15"/>
     </row>
-    <row r="25" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="9">
         <v>24</v>
       </c>
@@ -3169,9 +3149,8 @@
       <c r="AC25" s="15">
         <v>-6.1</v>
       </c>
-      <c r="AD25" s="15"/>
     </row>
-    <row r="26" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="9">
         <v>25</v>
       </c>
@@ -3259,9 +3238,8 @@
       <c r="AC26" s="15">
         <v>-6.1</v>
       </c>
-      <c r="AD26" s="15"/>
     </row>
-    <row r="27" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="9">
         <v>26</v>
       </c>
@@ -3353,9 +3331,8 @@
       <c r="AC27" s="15">
         <v>-5.7</v>
       </c>
-      <c r="AD27" s="15"/>
     </row>
-    <row r="28" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="9">
         <v>27</v>
       </c>
@@ -3447,9 +3424,8 @@
       <c r="AC28" s="15">
         <v>-5.3</v>
       </c>
-      <c r="AD28" s="15"/>
     </row>
-    <row r="29" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="9">
         <v>28</v>
       </c>
@@ -3541,9 +3517,8 @@
       <c r="AC29" s="15">
         <v>-5</v>
       </c>
-      <c r="AD29" s="15"/>
     </row>
-    <row r="30" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="9">
         <v>29</v>
       </c>
@@ -3635,9 +3610,8 @@
       <c r="AC30" s="15">
         <v>-5.9</v>
       </c>
-      <c r="AD30" s="15"/>
     </row>
-    <row r="31" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="9">
         <v>30</v>
       </c>
@@ -3729,9 +3703,8 @@
       <c r="AC31" s="15">
         <v>-5.7</v>
       </c>
-      <c r="AD31" s="15"/>
     </row>
-    <row r="32" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="9">
         <v>31</v>
       </c>
@@ -3823,9 +3796,8 @@
       <c r="AC32" s="15">
         <v>-5.6</v>
       </c>
-      <c r="AD32" s="15"/>
     </row>
-    <row r="33" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="9">
         <v>32</v>
       </c>
@@ -3917,9 +3889,8 @@
       <c r="AC33" s="15">
         <v>-5.7</v>
       </c>
-      <c r="AD33" s="15"/>
     </row>
-    <row r="34" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="9">
         <v>33</v>
       </c>
@@ -4009,9 +3980,8 @@
       <c r="AC34" s="15">
         <v>-5.5</v>
       </c>
-      <c r="AD34" s="15"/>
     </row>
-    <row r="35" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="9">
         <v>34</v>
       </c>
@@ -4103,9 +4073,8 @@
       <c r="AC35" s="15">
         <v>-5.7</v>
       </c>
-      <c r="AD35" s="15"/>
     </row>
-    <row r="36" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="9">
         <v>35</v>
       </c>
@@ -4197,9 +4166,8 @@
       <c r="AC36" s="15">
         <v>-5.7</v>
       </c>
-      <c r="AD36" s="15"/>
     </row>
-    <row r="37" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="9">
         <v>36</v>
       </c>
@@ -4291,9 +4259,8 @@
       <c r="AC37" s="15">
         <v>-5.8</v>
       </c>
-      <c r="AD37" s="15"/>
     </row>
-    <row r="38" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="9">
         <v>37</v>
       </c>
@@ -4385,9 +4352,8 @@
       <c r="AC38" s="15">
         <v>-5.9</v>
       </c>
-      <c r="AD38" s="15"/>
     </row>
-    <row r="39" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="9">
         <v>38</v>
       </c>
@@ -4479,9 +4445,8 @@
       <c r="AC39" s="15">
         <v>-5.6</v>
       </c>
-      <c r="AD39" s="15"/>
     </row>
-    <row r="40" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="9">
         <v>39</v>
       </c>
@@ -4573,9 +4538,8 @@
       <c r="AC40" s="15">
         <v>-6.3</v>
       </c>
-      <c r="AD40" s="15"/>
     </row>
-    <row r="41" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="9">
         <v>40</v>
       </c>
@@ -4667,9 +4631,8 @@
       <c r="AC41" s="15">
         <v>-5.3</v>
       </c>
-      <c r="AD41" s="15"/>
     </row>
-    <row r="42" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="9">
         <v>41</v>
       </c>
@@ -4761,9 +4724,8 @@
       <c r="AC42" s="15">
         <v>-5.9</v>
       </c>
-      <c r="AD42" s="15"/>
     </row>
-    <row r="43" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="9">
         <v>42</v>
       </c>
@@ -4855,9 +4817,8 @@
       <c r="AC43" s="15">
         <v>-5.3</v>
       </c>
-      <c r="AD43" s="15"/>
     </row>
-    <row r="44" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="9">
         <v>43</v>
       </c>
@@ -4947,9 +4908,8 @@
       <c r="AC44" s="15">
         <v>-6</v>
       </c>
-      <c r="AD44" s="15"/>
     </row>
-    <row r="45" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="9">
         <v>44</v>
       </c>
@@ -5041,9 +5001,8 @@
       <c r="AC45" s="15">
         <v>-5.8</v>
       </c>
-      <c r="AD45" s="15"/>
     </row>
-    <row r="46" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="9">
         <v>45</v>
       </c>
@@ -5135,9 +5094,8 @@
       <c r="AC46" s="15">
         <v>-6.2</v>
       </c>
-      <c r="AD46" s="15"/>
     </row>
-    <row r="47" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="9">
         <v>46</v>
       </c>
@@ -5229,9 +5187,8 @@
       <c r="AC47" s="15">
         <v>-5.0999999999999996</v>
       </c>
-      <c r="AD47" s="15"/>
     </row>
-    <row r="48" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48" s="9">
         <v>47</v>
       </c>
@@ -5323,9 +5280,8 @@
       <c r="AC48" s="15">
         <v>-5.0999999999999996</v>
       </c>
-      <c r="AD48" s="15"/>
     </row>
-    <row r="49" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A49" s="9">
         <v>48</v>
       </c>
@@ -5417,9 +5373,8 @@
       <c r="AC49" s="15">
         <v>-5.9</v>
       </c>
-      <c r="AD49" s="15"/>
     </row>
-    <row r="50" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A50" s="9">
         <v>49</v>
       </c>
@@ -5511,9 +5466,8 @@
       <c r="AC50" s="15">
         <v>-5.2</v>
       </c>
-      <c r="AD50" s="15"/>
     </row>
-    <row r="51" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A51" s="9">
         <v>50</v>
       </c>
@@ -5605,9 +5559,8 @@
       <c r="AC51" s="15">
         <v>-5.4</v>
       </c>
-      <c r="AD51" s="15"/>
     </row>
-    <row r="52" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A52" s="9">
         <v>51</v>
       </c>
@@ -5699,9 +5652,8 @@
       <c r="AC52" s="15">
         <v>-5.3</v>
       </c>
-      <c r="AD52" s="15"/>
     </row>
-    <row r="53" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A53" s="9">
         <v>52</v>
       </c>
@@ -5793,9 +5745,8 @@
       <c r="AC53" s="15">
         <v>-5.3</v>
       </c>
-      <c r="AD53" s="15"/>
     </row>
-    <row r="54" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A54" s="9">
         <v>53</v>
       </c>
@@ -5881,9 +5832,8 @@
       <c r="AC54" s="15">
         <v>-5.9</v>
       </c>
-      <c r="AD54" s="15"/>
     </row>
-    <row r="55" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A55" s="9">
         <v>54</v>
       </c>
@@ -5975,9 +5925,8 @@
       <c r="AC55" s="15">
         <v>-6.4</v>
       </c>
-      <c r="AD55" s="15"/>
     </row>
-    <row r="56" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A56" s="9">
         <v>55</v>
       </c>
@@ -6027,7 +5976,10 @@
       <c r="P56" s="15">
         <v>4.05</v>
       </c>
-      <c r="Q56" s="15"/>
+      <c r="Q56" s="15">
+        <f>T56</f>
+        <v>577</v>
+      </c>
       <c r="R56" s="15">
         <v>23.5</v>
       </c>
@@ -6067,9 +6019,8 @@
       <c r="AC56" s="15">
         <v>-6.1</v>
       </c>
-      <c r="AD56" s="15"/>
     </row>
-    <row r="57" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A57" s="9">
         <v>56</v>
       </c>
@@ -6161,9 +6112,8 @@
       <c r="AC57" s="15">
         <v>-5.0999999999999996</v>
       </c>
-      <c r="AD57" s="15"/>
     </row>
-    <row r="58" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A58" s="9">
         <v>57</v>
       </c>
@@ -6255,9 +6205,8 @@
       <c r="AC58" s="15">
         <v>-5.5</v>
       </c>
-      <c r="AD58" s="15"/>
     </row>
-    <row r="59" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A59" s="9">
         <v>58</v>
       </c>
@@ -6303,7 +6252,10 @@
         <v>12.29</v>
       </c>
       <c r="P59" s="15"/>
-      <c r="Q59" s="15"/>
+      <c r="Q59" s="15">
+        <f>T59</f>
+        <v>873</v>
+      </c>
       <c r="R59" s="15">
         <v>15.5</v>
       </c>
@@ -6343,9 +6295,8 @@
       <c r="AC59" s="15">
         <v>-4.0999999999999996</v>
       </c>
-      <c r="AD59" s="15"/>
     </row>
-    <row r="60" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A60" s="9">
         <v>59</v>
       </c>
@@ -6437,9 +6388,8 @@
       <c r="AC60" s="15">
         <v>-6</v>
       </c>
-      <c r="AD60" s="15"/>
     </row>
-    <row r="61" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A61" s="9">
         <v>60</v>
       </c>
@@ -6531,9 +6481,8 @@
       <c r="AC61" s="15">
         <v>-5</v>
       </c>
-      <c r="AD61" s="15"/>
     </row>
-    <row r="62" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A62" s="9">
         <v>61</v>
       </c>
@@ -6625,9 +6574,8 @@
       <c r="AC62" s="15">
         <v>-5.5</v>
       </c>
-      <c r="AD62" s="15"/>
     </row>
-    <row r="63" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A63" s="9">
         <v>62</v>
       </c>
@@ -6719,9 +6667,8 @@
       <c r="AC63" s="15">
         <v>-5.3</v>
       </c>
-      <c r="AD63" s="15"/>
     </row>
-    <row r="64" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="64" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A64" s="9">
         <v>63</v>
       </c>
@@ -6813,9 +6760,8 @@
       <c r="AC64" s="15">
         <v>-5.6</v>
       </c>
-      <c r="AD64" s="15"/>
     </row>
-    <row r="65" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A65" s="9">
         <v>64</v>
       </c>
@@ -6907,9 +6853,8 @@
       <c r="AC65" s="15">
         <v>-5.8</v>
       </c>
-      <c r="AD65" s="15"/>
     </row>
-    <row r="66" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A66" s="9">
         <v>65</v>
       </c>
@@ -6999,9 +6944,8 @@
       <c r="AC66" s="15">
         <v>-5.5</v>
       </c>
-      <c r="AD66" s="15"/>
     </row>
-    <row r="67" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A67" s="9">
         <v>66</v>
       </c>
@@ -7051,7 +6995,10 @@
       <c r="P67" s="15">
         <v>3.97</v>
       </c>
-      <c r="Q67" s="15"/>
+      <c r="Q67" s="15">
+        <f>T67</f>
+        <v>679</v>
+      </c>
       <c r="R67" s="15">
         <v>14</v>
       </c>
@@ -7091,9 +7038,8 @@
       <c r="AC67" s="15">
         <v>-5.2</v>
       </c>
-      <c r="AD67" s="15"/>
     </row>
-    <row r="68" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A68" s="9">
         <v>67</v>
       </c>
@@ -7143,7 +7089,10 @@
       <c r="P68" s="15">
         <v>3.88</v>
       </c>
-      <c r="Q68" s="15"/>
+      <c r="Q68" s="15">
+        <f>T68</f>
+        <v>686</v>
+      </c>
       <c r="R68" s="15">
         <v>11</v>
       </c>
@@ -7183,9 +7132,8 @@
       <c r="AC68" s="15">
         <v>-5.2</v>
       </c>
-      <c r="AD68" s="15"/>
     </row>
-    <row r="69" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A69" s="9">
         <v>68</v>
       </c>
@@ -7277,9 +7225,8 @@
       <c r="AC69" s="15">
         <v>-5.2</v>
       </c>
-      <c r="AD69" s="15"/>
     </row>
-    <row r="70" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A70" s="9">
         <v>69</v>
       </c>
@@ -7329,7 +7276,10 @@
       <c r="P70" s="15">
         <v>4.84</v>
       </c>
-      <c r="Q70" s="15"/>
+      <c r="Q70" s="15">
+        <f>T70</f>
+        <v>592</v>
+      </c>
       <c r="R70" s="15">
         <v>12</v>
       </c>
@@ -7369,9 +7319,8 @@
       <c r="AC70" s="15">
         <v>-6</v>
       </c>
-      <c r="AD70" s="15"/>
     </row>
-    <row r="71" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A71" s="9">
         <v>70</v>
       </c>
@@ -7463,9 +7412,8 @@
       <c r="AC71" s="15">
         <v>-5.9</v>
       </c>
-      <c r="AD71" s="15"/>
     </row>
-    <row r="72" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A72" s="9">
         <v>71</v>
       </c>
@@ -7555,9 +7503,8 @@
       <c r="AC72" s="15">
         <v>-6</v>
       </c>
-      <c r="AD72" s="15"/>
     </row>
-    <row r="73" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A73" s="9">
         <v>72</v>
       </c>
@@ -7649,9 +7596,8 @@
       <c r="AC73" s="15">
         <v>-5.4</v>
       </c>
-      <c r="AD73" s="15"/>
     </row>
-    <row r="74" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A74" s="9">
         <v>73</v>
       </c>
@@ -7743,11 +7689,8 @@
       <c r="AC74" s="15">
         <v>-6.3</v>
       </c>
-      <c r="AD74" s="15" t="s">
-        <v>104</v>
-      </c>
     </row>
-    <row r="75" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A75" s="9">
         <v>74</v>
       </c>
@@ -7839,9 +7782,8 @@
       <c r="AC75" s="15">
         <v>-5.7</v>
       </c>
-      <c r="AD75" s="15"/>
     </row>
-    <row r="76" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A76" s="9">
         <v>75</v>
       </c>
@@ -7891,7 +7833,10 @@
       <c r="P76" s="15">
         <v>4.58</v>
       </c>
-      <c r="Q76" s="15"/>
+      <c r="Q76" s="15">
+        <f>T76</f>
+        <v>673</v>
+      </c>
       <c r="R76" s="15">
         <v>13</v>
       </c>
@@ -7931,9 +7876,8 @@
       <c r="AC76" s="15">
         <v>-5.5</v>
       </c>
-      <c r="AD76" s="15"/>
     </row>
-    <row r="77" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A77" s="9">
         <v>76</v>
       </c>
@@ -7983,7 +7927,10 @@
       <c r="P77" s="15">
         <v>4.3899999999999997</v>
       </c>
-      <c r="Q77" s="15"/>
+      <c r="Q77" s="15">
+        <f>T77</f>
+        <v>797</v>
+      </c>
       <c r="R77" s="15">
         <v>30</v>
       </c>
@@ -8023,9 +7970,8 @@
       <c r="AC77" s="15">
         <v>-6.2</v>
       </c>
-      <c r="AD77" s="15"/>
     </row>
-    <row r="78" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A78" s="9">
         <v>77</v>
       </c>
@@ -8117,9 +8063,8 @@
       <c r="AC78" s="15">
         <v>-5.5</v>
       </c>
-      <c r="AD78" s="15"/>
     </row>
-    <row r="79" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A79" s="9">
         <v>78</v>
       </c>
@@ -8211,9 +8156,8 @@
       <c r="AC79" s="15">
         <v>-5.6</v>
       </c>
-      <c r="AD79" s="15"/>
     </row>
-    <row r="80" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="80" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A80" s="9">
         <v>79</v>
       </c>
@@ -8263,7 +8207,10 @@
       <c r="P80" s="15">
         <v>5.05</v>
       </c>
-      <c r="Q80" s="15"/>
+      <c r="Q80" s="15">
+        <f>T80</f>
+        <v>724</v>
+      </c>
       <c r="R80" s="15">
         <v>23.5</v>
       </c>
@@ -8303,9 +8250,8 @@
       <c r="AC80" s="15">
         <v>-5.2</v>
       </c>
-      <c r="AD80" s="15"/>
     </row>
-    <row r="81" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="81" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A81" s="9">
         <v>80</v>
       </c>
@@ -8322,7 +8268,7 @@
         <v>20607</v>
       </c>
       <c r="F81" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G81" s="13">
         <v>44755</v>
@@ -8353,7 +8299,10 @@
       <c r="P81" s="15">
         <v>4.5599999999999996</v>
       </c>
-      <c r="Q81" s="15"/>
+      <c r="Q81" s="15">
+        <f>T81</f>
+        <v>745</v>
+      </c>
       <c r="R81" s="15">
         <v>24</v>
       </c>
@@ -8393,9 +8342,8 @@
       <c r="AC81" s="15">
         <v>-5.4</v>
       </c>
-      <c r="AD81" s="15"/>
     </row>
-    <row r="82" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="82" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A82" s="9">
         <v>81</v>
       </c>
@@ -8487,9 +8435,8 @@
       <c r="AC82" s="15">
         <v>-5.3</v>
       </c>
-      <c r="AD82" s="15"/>
     </row>
-    <row r="83" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="83" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A83" s="9">
         <v>82</v>
       </c>
@@ -8581,9 +8528,8 @@
       <c r="AC83" s="15">
         <v>-5.7</v>
       </c>
-      <c r="AD83" s="15"/>
     </row>
-    <row r="84" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="84" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A84" s="9">
         <v>83</v>
       </c>
@@ -8633,7 +8579,10 @@
       <c r="P84" s="15">
         <v>5.56</v>
       </c>
-      <c r="Q84" s="15"/>
+      <c r="Q84" s="15">
+        <f>T84</f>
+        <v>509</v>
+      </c>
       <c r="R84" s="15">
         <v>19.5</v>
       </c>
@@ -8673,9 +8622,8 @@
       <c r="AC84" s="15">
         <v>-5.3</v>
       </c>
-      <c r="AD84" s="15"/>
     </row>
-    <row r="85" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="85" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A85" s="9">
         <v>84</v>
       </c>
@@ -8767,9 +8715,8 @@
       <c r="AC85" s="15">
         <v>-5.5</v>
       </c>
-      <c r="AD85" s="15"/>
     </row>
-    <row r="86" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="86" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A86" s="9">
         <v>85</v>
       </c>
@@ -8861,9 +8808,8 @@
       <c r="AC86" s="15">
         <v>-5.8</v>
       </c>
-      <c r="AD86" s="15"/>
     </row>
-    <row r="87" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="87" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A87" s="9">
         <v>86</v>
       </c>
@@ -8913,7 +8859,10 @@
       <c r="P87" s="15">
         <v>5.47</v>
       </c>
-      <c r="Q87" s="15"/>
+      <c r="Q87" s="15">
+        <f>T87</f>
+        <v>705</v>
+      </c>
       <c r="R87" s="15">
         <v>26</v>
       </c>
@@ -8953,9 +8902,8 @@
       <c r="AC87" s="15">
         <v>-6.1</v>
       </c>
-      <c r="AD87" s="15"/>
     </row>
-    <row r="88" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="88" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A88" s="9">
         <v>87</v>
       </c>
@@ -9047,9 +8995,8 @@
       <c r="AC88" s="15">
         <v>-6.2</v>
       </c>
-      <c r="AD88" s="15"/>
     </row>
-    <row r="89" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="89" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A89" s="9">
         <v>88</v>
       </c>
@@ -9141,9 +9088,8 @@
       <c r="AC89" s="15">
         <v>-6</v>
       </c>
-      <c r="AD89" s="15"/>
     </row>
-    <row r="90" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="90" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A90" s="9">
         <v>89</v>
       </c>
@@ -9235,9 +9181,8 @@
       <c r="AC90" s="15">
         <v>-6.1</v>
       </c>
-      <c r="AD90" s="15"/>
     </row>
-    <row r="91" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="91" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A91" s="9">
         <v>90</v>
       </c>
@@ -9325,9 +9270,8 @@
       <c r="AC91" s="15">
         <v>-5.3</v>
       </c>
-      <c r="AD91" s="15"/>
     </row>
-    <row r="92" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="92" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A92" s="9">
         <v>91</v>
       </c>
@@ -9419,9 +9363,8 @@
       <c r="AC92" s="15">
         <v>-5.5</v>
       </c>
-      <c r="AD92" s="15"/>
     </row>
-    <row r="93" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="93" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A93" s="9">
         <v>92</v>
       </c>
@@ -9513,9 +9456,8 @@
       <c r="AC93" s="15">
         <v>-5.7</v>
       </c>
-      <c r="AD93" s="15"/>
     </row>
-    <row r="94" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="94" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A94" s="9">
         <v>93</v>
       </c>
@@ -9565,7 +9507,10 @@
       <c r="P94" s="15">
         <v>4.78</v>
       </c>
-      <c r="Q94" s="15"/>
+      <c r="Q94" s="15">
+        <f>T94</f>
+        <v>579</v>
+      </c>
       <c r="R94" s="15">
         <v>27</v>
       </c>
@@ -9605,9 +9550,8 @@
       <c r="AC94" s="15">
         <v>-5.5</v>
       </c>
-      <c r="AD94" s="15"/>
     </row>
-    <row r="95" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="95" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A95" s="9">
         <v>94</v>
       </c>
@@ -9699,9 +9643,8 @@
       <c r="AC95" s="15">
         <v>-5.4</v>
       </c>
-      <c r="AD95" s="15"/>
     </row>
-    <row r="96" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="96" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A96" s="9">
         <v>95</v>
       </c>
@@ -9793,9 +9736,8 @@
       <c r="AC96" s="15">
         <v>-5.5</v>
       </c>
-      <c r="AD96" s="15"/>
     </row>
-    <row r="97" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="97" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A97" s="9">
         <v>96</v>
       </c>
@@ -9887,9 +9829,8 @@
       <c r="AC97" s="15">
         <v>-6.3</v>
       </c>
-      <c r="AD97" s="15"/>
     </row>
-    <row r="98" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="98" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A98" s="9">
         <v>97</v>
       </c>
@@ -9939,7 +9880,10 @@
       <c r="P98" s="15">
         <v>4.2699999999999996</v>
       </c>
-      <c r="Q98" s="15"/>
+      <c r="Q98" s="15">
+        <f>T98</f>
+        <v>880</v>
+      </c>
       <c r="R98" s="15">
         <v>28</v>
       </c>
@@ -9979,10 +9923,9 @@
       <c r="AC98" s="15">
         <v>-5.8</v>
       </c>
-      <c r="AD98" s="15"/>
     </row>
   </sheetData>
-  <autoFilter ref="B1:AD98" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="B1:AC98" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>

</xml_diff>

<commit_message>
Remove temporary file ~$FacoDMEK.xlsx
</commit_message>
<xml_diff>
--- a/FacoDMEK.xlsx
+++ b/FacoDMEK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Websites\faco-dmek\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A48D2B0B-6E74-4600-B9C7-2544AA1D9D37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FDD6C90-A6B3-4C88-988C-18E016B284B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -820,10 +820,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="Q99" sqref="Q99"/>
+      <selection pane="bottomLeft" activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.2109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -3185,8 +3185,12 @@
       <c r="K26" s="15">
         <v>27.48</v>
       </c>
-      <c r="L26" s="15"/>
-      <c r="M26" s="15"/>
+      <c r="L26" s="15">
+        <v>41.2</v>
+      </c>
+      <c r="M26" s="15">
+        <v>39.4</v>
+      </c>
       <c r="N26" s="15">
         <v>2.8</v>
       </c>
@@ -5816,12 +5820,16 @@
       <c r="W54" s="15">
         <v>44.5</v>
       </c>
-      <c r="X54" s="16" t="e">
+      <c r="X54" s="16">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y54" s="15"/>
-      <c r="Z54" s="15"/>
+        <v>44.585000000000001</v>
+      </c>
+      <c r="Y54" s="15">
+        <v>44.7</v>
+      </c>
+      <c r="Z54" s="15">
+        <v>44.47</v>
+      </c>
       <c r="AA54" s="16">
         <f t="shared" si="3"/>
         <v>-6</v>

</xml_diff>

<commit_message>
Add FacoDMEK data processing notebook and remove temporary files
</commit_message>
<xml_diff>
--- a/FacoDMEK.xlsx
+++ b/FacoDMEK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Websites\faco-dmek\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FDD6C90-A6B3-4C88-988C-18E016B284B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A296C332-95B3-4D0F-A33C-675CDBB79F98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -820,10 +820,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="P20" sqref="P20"/>
+      <selection pane="bottomLeft" activeCell="N60" sqref="N60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.2109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -1989,7 +1989,9 @@
       <c r="M13" s="15">
         <v>46.26</v>
       </c>
-      <c r="N13" s="15"/>
+      <c r="N13" s="15">
+        <v>2.09</v>
+      </c>
       <c r="O13" s="15">
         <v>11.99</v>
       </c>
@@ -2637,7 +2639,9 @@
       <c r="M20" s="15">
         <v>44.2</v>
       </c>
-      <c r="N20" s="15"/>
+      <c r="N20" s="15">
+        <v>2.21</v>
+      </c>
       <c r="O20" s="15">
         <v>12.64</v>
       </c>
@@ -6255,7 +6259,9 @@
       <c r="M59" s="15">
         <v>43.5</v>
       </c>
-      <c r="N59" s="15"/>
+      <c r="N59" s="15">
+        <v>2.61</v>
+      </c>
       <c r="O59" s="15">
         <v>12.29</v>
       </c>

</xml_diff>

<commit_message>
Update FacoDMEK data processing results and remove temporary files
</commit_message>
<xml_diff>
--- a/FacoDMEK.xlsx
+++ b/FacoDMEK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Websites\faco-dmek\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A296C332-95B3-4D0F-A33C-675CDBB79F98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CEC0E65-8C4D-4519-9831-84C2EB2B78D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -393,7 +393,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -408,6 +408,13 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -471,7 +478,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -519,6 +526,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -821,9 +831,9 @@
   <dimension ref="A1:AC98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="N60" sqref="N60"/>
+      <selection pane="bottomLeft" activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.2109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -1160,7 +1170,9 @@
       <c r="O4" s="15">
         <v>11.71</v>
       </c>
-      <c r="P4" s="15"/>
+      <c r="P4" s="15">
+        <v>4.5599999999999996</v>
+      </c>
       <c r="Q4" s="15">
         <v>649</v>
       </c>
@@ -2551,7 +2563,9 @@
       <c r="N19" s="15">
         <v>3.04</v>
       </c>
-      <c r="O19" s="15"/>
+      <c r="O19" s="15">
+        <v>11.76</v>
+      </c>
       <c r="P19" s="15">
         <v>4.8899999999999997</v>
       </c>
@@ -2645,7 +2659,9 @@
       <c r="O20" s="15">
         <v>12.64</v>
       </c>
-      <c r="P20" s="15"/>
+      <c r="P20" s="15">
+        <v>4.8899999999999997</v>
+      </c>
       <c r="Q20" s="15">
         <v>668</v>
       </c>
@@ -3945,7 +3961,9 @@
       <c r="O34" s="15">
         <v>11.7</v>
       </c>
-      <c r="P34" s="15"/>
+      <c r="P34" s="15">
+        <v>4.74</v>
+      </c>
       <c r="Q34" s="15">
         <v>662</v>
       </c>
@@ -4873,7 +4891,9 @@
       <c r="O44" s="15">
         <v>11.34</v>
       </c>
-      <c r="P44" s="15"/>
+      <c r="P44" s="15">
+        <v>4.83</v>
+      </c>
       <c r="Q44" s="15">
         <v>560</v>
       </c>
@@ -5798,7 +5818,9 @@
       <c r="N54" s="15">
         <v>3.16</v>
       </c>
-      <c r="O54" s="15"/>
+      <c r="O54" s="15">
+        <v>11.77</v>
+      </c>
       <c r="P54" s="15">
         <v>4.6399999999999997</v>
       </c>
@@ -6179,7 +6201,7 @@
         <v>588</v>
       </c>
       <c r="R58" s="15">
-        <v>0.74305555555555558</v>
+        <v>27</v>
       </c>
       <c r="S58" s="15">
         <v>119.1</v>
@@ -6265,7 +6287,9 @@
       <c r="O59" s="15">
         <v>12.29</v>
       </c>
-      <c r="P59" s="15"/>
+      <c r="P59" s="15">
+        <v>4.83</v>
+      </c>
       <c r="Q59" s="15">
         <f>T59</f>
         <v>873</v>
@@ -6912,7 +6936,9 @@
       <c r="N66" s="15">
         <v>3.41</v>
       </c>
-      <c r="O66" s="15"/>
+      <c r="O66" s="15">
+        <v>12.01</v>
+      </c>
       <c r="P66" s="15">
         <v>4.66</v>
       </c>
@@ -7474,7 +7500,9 @@
       <c r="O72" s="15">
         <v>12.76</v>
       </c>
-      <c r="P72" s="15"/>
+      <c r="P72" s="15">
+        <v>4.5199999999999996</v>
+      </c>
       <c r="Q72" s="15">
         <v>544</v>
       </c>
@@ -8309,7 +8337,9 @@
       <c r="N81" s="15">
         <v>2.48</v>
       </c>
-      <c r="O81" s="15"/>
+      <c r="O81" s="15">
+        <v>11.77</v>
+      </c>
       <c r="P81" s="15">
         <v>4.5599999999999996</v>
       </c>
@@ -9240,8 +9270,12 @@
       <c r="N91" s="15">
         <v>3</v>
       </c>
-      <c r="O91" s="15"/>
-      <c r="P91" s="15"/>
+      <c r="O91" s="15">
+        <v>11.87</v>
+      </c>
+      <c r="P91" s="15">
+        <v>4.62</v>
+      </c>
       <c r="Q91" s="15">
         <v>463</v>
       </c>
@@ -9329,7 +9363,7 @@
       <c r="N92" s="15">
         <v>3.06</v>
       </c>
-      <c r="O92" s="15">
+      <c r="O92" s="17">
         <v>12.01</v>
       </c>
       <c r="P92" s="15">

</xml_diff>

<commit_message>
Update FacoDMEK.xlsx with new data
</commit_message>
<xml_diff>
--- a/FacoDMEK.xlsx
+++ b/FacoDMEK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Websites\faco-dmek\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CEC0E65-8C4D-4519-9831-84C2EB2B78D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42182927-20E1-46DA-8645-BB9F42D57FBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -830,10 +830,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="H58" sqref="H58"/>
+      <selection pane="bottomLeft" activeCell="S44" sqref="S44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.2109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -959,7 +959,6 @@
         <v>44531</v>
       </c>
       <c r="H2" s="14">
-        <f t="shared" ref="H2:H98" si="0">INT(YEARFRAC(E2,G2))</f>
         <v>67</v>
       </c>
       <c r="I2" s="15">
@@ -987,7 +986,6 @@
         <v>4.0599999999999996</v>
       </c>
       <c r="Q2" s="15">
-        <f>T2</f>
         <v>594</v>
       </c>
       <c r="R2" s="15">
@@ -1000,7 +998,6 @@
         <v>594</v>
       </c>
       <c r="U2" s="16">
-        <f t="shared" ref="U2:U98" si="1">AVERAGE(V2:W2)</f>
         <v>45.7</v>
       </c>
       <c r="V2" s="15">
@@ -1010,7 +1007,6 @@
         <v>44.9</v>
       </c>
       <c r="X2" s="16">
-        <f t="shared" ref="X2:X98" si="2">AVERAGE(Y2:Z2)</f>
         <v>50.9</v>
       </c>
       <c r="Y2" s="15">
@@ -1020,7 +1016,6 @@
         <v>50</v>
       </c>
       <c r="AA2" s="16">
-        <f t="shared" ref="AA2:AA98" si="3">AVERAGE(AB2:AC2)</f>
         <v>-6.45</v>
       </c>
       <c r="AB2" s="15">
@@ -1053,7 +1048,6 @@
         <v>44230</v>
       </c>
       <c r="H3" s="14">
-        <f t="shared" si="0"/>
         <v>53</v>
       </c>
       <c r="I3" s="15">
@@ -1093,7 +1087,6 @@
         <v>699</v>
       </c>
       <c r="U3" s="16">
-        <f t="shared" si="1"/>
         <v>47.2</v>
       </c>
       <c r="V3" s="15">
@@ -1103,7 +1096,6 @@
         <v>46.4</v>
       </c>
       <c r="X3" s="16">
-        <f t="shared" si="2"/>
         <v>52.6</v>
       </c>
       <c r="Y3" s="15">
@@ -1113,7 +1105,6 @@
         <v>51.7</v>
       </c>
       <c r="AA3" s="16">
-        <f t="shared" si="3"/>
         <v>-6.6</v>
       </c>
       <c r="AB3" s="15">
@@ -1146,7 +1137,6 @@
         <v>44006</v>
       </c>
       <c r="H4" s="14">
-        <f t="shared" si="0"/>
         <v>69</v>
       </c>
       <c r="I4" s="15">
@@ -1186,7 +1176,6 @@
         <v>663</v>
       </c>
       <c r="U4" s="16">
-        <f t="shared" si="1"/>
         <v>40.700000000000003</v>
       </c>
       <c r="V4" s="15">
@@ -1196,7 +1185,6 @@
         <v>40.5</v>
       </c>
       <c r="X4" s="16">
-        <f t="shared" si="2"/>
         <v>45.3</v>
       </c>
       <c r="Y4" s="15">
@@ -1206,7 +1194,6 @@
         <v>45.1</v>
       </c>
       <c r="AA4" s="16">
-        <f t="shared" si="3"/>
         <v>-6.6</v>
       </c>
       <c r="AB4" s="15">
@@ -1239,7 +1226,6 @@
         <v>44468</v>
       </c>
       <c r="H5" s="14">
-        <f t="shared" si="0"/>
         <v>74</v>
       </c>
       <c r="I5" s="15">
@@ -1279,7 +1265,6 @@
         <v>526</v>
       </c>
       <c r="U5" s="16">
-        <f t="shared" si="1"/>
         <v>43.25</v>
       </c>
       <c r="V5" s="15">
@@ -1289,7 +1274,6 @@
         <v>43</v>
       </c>
       <c r="X5" s="16">
-        <f t="shared" si="2"/>
         <v>48.2</v>
       </c>
       <c r="Y5" s="15">
@@ -1299,7 +1283,6 @@
         <v>47.9</v>
       </c>
       <c r="AA5" s="16">
-        <f t="shared" si="3"/>
         <v>-5.6</v>
       </c>
       <c r="AB5" s="15">
@@ -1332,7 +1315,6 @@
         <v>44132</v>
       </c>
       <c r="H6" s="14">
-        <f t="shared" si="0"/>
         <v>79</v>
       </c>
       <c r="I6" s="15">
@@ -1372,7 +1354,6 @@
         <v>603</v>
       </c>
       <c r="U6" s="16">
-        <f t="shared" si="1"/>
         <v>43.7</v>
       </c>
       <c r="V6" s="15">
@@ -1382,7 +1363,6 @@
         <v>42.8</v>
       </c>
       <c r="X6" s="16">
-        <f t="shared" si="2"/>
         <v>48.7</v>
       </c>
       <c r="Y6" s="15">
@@ -1392,7 +1372,6 @@
         <v>47.7</v>
       </c>
       <c r="AA6" s="16">
-        <f t="shared" si="3"/>
         <v>-5.8000000000000007</v>
       </c>
       <c r="AB6" s="15">
@@ -1425,7 +1404,6 @@
         <v>44167</v>
       </c>
       <c r="H7" s="14">
-        <f t="shared" si="0"/>
         <v>75</v>
       </c>
       <c r="I7" s="15">
@@ -1465,7 +1443,6 @@
         <v>652</v>
       </c>
       <c r="U7" s="16">
-        <f t="shared" si="1"/>
         <v>43.85</v>
       </c>
       <c r="V7" s="15">
@@ -1475,7 +1452,6 @@
         <v>43.6</v>
       </c>
       <c r="X7" s="16">
-        <f t="shared" si="2"/>
         <v>48.85</v>
       </c>
       <c r="Y7" s="15">
@@ -1485,7 +1461,6 @@
         <v>48.6</v>
       </c>
       <c r="AA7" s="16">
-        <f t="shared" si="3"/>
         <v>-5.7</v>
       </c>
       <c r="AB7" s="15">
@@ -1518,7 +1493,6 @@
         <v>44160</v>
       </c>
       <c r="H8" s="14">
-        <f t="shared" si="0"/>
         <v>67</v>
       </c>
       <c r="I8" s="15">
@@ -1558,7 +1532,6 @@
         <v>607</v>
       </c>
       <c r="U8" s="16">
-        <f t="shared" si="1"/>
         <v>43.8</v>
       </c>
       <c r="V8" s="15">
@@ -1568,7 +1541,6 @@
         <v>42.9</v>
       </c>
       <c r="X8" s="16">
-        <f t="shared" si="2"/>
         <v>48.8</v>
       </c>
       <c r="Y8" s="15">
@@ -1578,7 +1550,6 @@
         <v>47.8</v>
       </c>
       <c r="AA8" s="16">
-        <f t="shared" si="3"/>
         <v>-5.9499999999999993</v>
       </c>
       <c r="AB8" s="15">
@@ -1611,7 +1582,6 @@
         <v>44256</v>
       </c>
       <c r="H9" s="14">
-        <f t="shared" si="0"/>
         <v>67</v>
       </c>
       <c r="I9" s="15">
@@ -1651,7 +1621,6 @@
         <v>612</v>
       </c>
       <c r="U9" s="16">
-        <f t="shared" si="1"/>
         <v>44.05</v>
       </c>
       <c r="V9" s="15">
@@ -1661,7 +1630,6 @@
         <v>43.2</v>
       </c>
       <c r="X9" s="16">
-        <f t="shared" si="2"/>
         <v>49.1</v>
       </c>
       <c r="Y9" s="15">
@@ -1671,7 +1639,6 @@
         <v>48.1</v>
       </c>
       <c r="AA9" s="16">
-        <f t="shared" si="3"/>
         <v>-5.85</v>
       </c>
       <c r="AB9" s="15">
@@ -1704,7 +1671,6 @@
         <v>45035</v>
       </c>
       <c r="H10" s="14">
-        <f t="shared" si="0"/>
         <v>68</v>
       </c>
       <c r="I10" s="15">
@@ -1744,7 +1710,6 @@
         <v>659</v>
       </c>
       <c r="U10" s="16">
-        <f t="shared" si="1"/>
         <v>46.25</v>
       </c>
       <c r="V10" s="15">
@@ -1754,7 +1719,6 @@
         <v>45.9</v>
       </c>
       <c r="X10" s="16">
-        <f t="shared" si="2"/>
         <v>51.5</v>
       </c>
       <c r="Y10" s="15">
@@ -1764,7 +1728,6 @@
         <v>51.1</v>
       </c>
       <c r="AA10" s="16">
-        <f t="shared" si="3"/>
         <v>-5.6999999999999993</v>
       </c>
       <c r="AB10" s="15">
@@ -1797,7 +1760,6 @@
         <v>44286</v>
       </c>
       <c r="H11" s="14">
-        <f t="shared" si="0"/>
         <v>70</v>
       </c>
       <c r="I11" s="15">
@@ -1837,7 +1799,6 @@
         <v>549</v>
       </c>
       <c r="U11" s="16">
-        <f t="shared" si="1"/>
         <v>43.900000000000006</v>
       </c>
       <c r="V11" s="15">
@@ -1847,7 +1808,6 @@
         <v>43.2</v>
       </c>
       <c r="X11" s="16">
-        <f t="shared" si="2"/>
         <v>48.900000000000006</v>
       </c>
       <c r="Y11" s="15">
@@ -1857,7 +1817,6 @@
         <v>48.1</v>
       </c>
       <c r="AA11" s="16">
-        <f t="shared" si="3"/>
         <v>-6</v>
       </c>
       <c r="AB11" s="15">
@@ -1890,7 +1849,6 @@
         <v>44461</v>
       </c>
       <c r="H12" s="14">
-        <f t="shared" si="0"/>
         <v>71</v>
       </c>
       <c r="I12" s="15">
@@ -1930,7 +1888,6 @@
         <v>552</v>
       </c>
       <c r="U12" s="16">
-        <f t="shared" si="1"/>
         <v>43.7</v>
       </c>
       <c r="V12" s="15">
@@ -1940,7 +1897,6 @@
         <v>41.6</v>
       </c>
       <c r="X12" s="16">
-        <f t="shared" si="2"/>
         <v>48.7</v>
       </c>
       <c r="Y12" s="15">
@@ -1950,7 +1906,6 @@
         <v>46.4</v>
       </c>
       <c r="AA12" s="16">
-        <f t="shared" si="3"/>
         <v>-5.8</v>
       </c>
       <c r="AB12" s="15">
@@ -1983,7 +1938,6 @@
         <v>44146</v>
       </c>
       <c r="H13" s="14">
-        <f t="shared" si="0"/>
         <v>58</v>
       </c>
       <c r="I13" s="15">
@@ -2023,7 +1977,6 @@
         <v>816</v>
       </c>
       <c r="U13" s="16">
-        <f t="shared" si="1"/>
         <v>46.400000000000006</v>
       </c>
       <c r="V13" s="15">
@@ -2033,7 +1986,6 @@
         <v>46.2</v>
       </c>
       <c r="X13" s="16">
-        <f t="shared" si="2"/>
         <v>51.7</v>
       </c>
       <c r="Y13" s="15">
@@ -2043,7 +1995,6 @@
         <v>51.5</v>
       </c>
       <c r="AA13" s="16">
-        <f t="shared" si="3"/>
         <v>-5.15</v>
       </c>
       <c r="AB13" s="15">
@@ -2076,7 +2027,6 @@
         <v>44209</v>
       </c>
       <c r="H14" s="14">
-        <f t="shared" si="0"/>
         <v>73</v>
       </c>
       <c r="I14" s="15">
@@ -2116,7 +2066,6 @@
         <v>600</v>
       </c>
       <c r="U14" s="16">
-        <f t="shared" si="1"/>
         <v>42.45</v>
       </c>
       <c r="V14" s="15">
@@ -2126,7 +2075,6 @@
         <v>41.3</v>
       </c>
       <c r="X14" s="16">
-        <f t="shared" si="2"/>
         <v>47.35</v>
       </c>
       <c r="Y14" s="15">
@@ -2136,7 +2084,6 @@
         <v>46.1</v>
       </c>
       <c r="AA14" s="16">
-        <f t="shared" si="3"/>
         <v>-5.7</v>
       </c>
       <c r="AB14" s="15">
@@ -2169,7 +2116,6 @@
         <v>44951</v>
       </c>
       <c r="H15" s="14">
-        <f t="shared" si="0"/>
         <v>67</v>
       </c>
       <c r="I15" s="15">
@@ -2209,7 +2155,6 @@
         <v>531</v>
       </c>
       <c r="U15" s="16">
-        <f t="shared" si="1"/>
         <v>42.349999999999994</v>
       </c>
       <c r="V15" s="15">
@@ -2219,7 +2164,6 @@
         <v>41.9</v>
       </c>
       <c r="X15" s="16">
-        <f t="shared" si="2"/>
         <v>47.150000000000006</v>
       </c>
       <c r="Y15" s="15">
@@ -2229,7 +2173,6 @@
         <v>46.7</v>
       </c>
       <c r="AA15" s="16">
-        <f t="shared" si="3"/>
         <v>-5.9499999999999993</v>
       </c>
       <c r="AB15" s="15">
@@ -2262,7 +2205,6 @@
         <v>45091</v>
       </c>
       <c r="H16" s="14">
-        <f t="shared" si="0"/>
         <v>68</v>
       </c>
       <c r="I16" s="15">
@@ -2302,7 +2244,6 @@
         <v>589</v>
       </c>
       <c r="U16" s="16">
-        <f t="shared" si="1"/>
         <v>42.25</v>
       </c>
       <c r="V16" s="15">
@@ -2312,7 +2253,6 @@
         <v>41.7</v>
       </c>
       <c r="X16" s="16">
-        <f t="shared" si="2"/>
         <v>47.05</v>
       </c>
       <c r="Y16" s="15">
@@ -2322,7 +2262,6 @@
         <v>46.5</v>
       </c>
       <c r="AA16" s="16">
-        <f t="shared" si="3"/>
         <v>-5.7</v>
       </c>
       <c r="AB16" s="15">
@@ -2355,7 +2294,6 @@
         <v>44846</v>
       </c>
       <c r="H17" s="14">
-        <f t="shared" si="0"/>
         <v>69</v>
       </c>
       <c r="I17" s="15">
@@ -2383,7 +2321,6 @@
         <v>4.8099999999999996</v>
       </c>
       <c r="Q17" s="15">
-        <f>T17</f>
         <v>638</v>
       </c>
       <c r="R17" s="15">
@@ -2396,7 +2333,6 @@
         <v>638</v>
       </c>
       <c r="U17" s="16">
-        <f t="shared" si="1"/>
         <v>43.55</v>
       </c>
       <c r="V17" s="15">
@@ -2406,7 +2342,6 @@
         <v>42.7</v>
       </c>
       <c r="X17" s="16">
-        <f t="shared" si="2"/>
         <v>48.45</v>
       </c>
       <c r="Y17" s="15">
@@ -2416,7 +2351,6 @@
         <v>47.5</v>
       </c>
       <c r="AA17" s="16">
-        <f t="shared" si="3"/>
         <v>-5.65</v>
       </c>
       <c r="AB17" s="15">
@@ -2449,7 +2383,6 @@
         <v>44993</v>
       </c>
       <c r="H18" s="14">
-        <f t="shared" si="0"/>
         <v>53</v>
       </c>
       <c r="I18" s="15">
@@ -2489,7 +2422,6 @@
         <v>541</v>
       </c>
       <c r="U18" s="16">
-        <f t="shared" si="1"/>
         <v>47.25</v>
       </c>
       <c r="V18" s="15">
@@ -2499,7 +2431,6 @@
         <v>46.2</v>
       </c>
       <c r="X18" s="16">
-        <f t="shared" si="2"/>
         <v>52.65</v>
       </c>
       <c r="Y18" s="15">
@@ -2509,7 +2440,6 @@
         <v>51.5</v>
       </c>
       <c r="AA18" s="16">
-        <f t="shared" si="3"/>
         <v>-6.35</v>
       </c>
       <c r="AB18" s="15">
@@ -2542,7 +2472,6 @@
         <v>45384</v>
       </c>
       <c r="H19" s="14">
-        <f t="shared" si="0"/>
         <v>66</v>
       </c>
       <c r="I19" s="15">
@@ -2582,7 +2511,6 @@
         <v>602</v>
       </c>
       <c r="U19" s="16">
-        <f t="shared" si="1"/>
         <v>43.9</v>
       </c>
       <c r="V19" s="15">
@@ -2592,7 +2520,6 @@
         <v>43.4</v>
       </c>
       <c r="X19" s="16">
-        <f t="shared" si="2"/>
         <v>48.95</v>
       </c>
       <c r="Y19" s="15">
@@ -2602,7 +2529,6 @@
         <v>48.4</v>
       </c>
       <c r="AA19" s="16">
-        <f t="shared" si="3"/>
         <v>-5.4</v>
       </c>
       <c r="AB19" s="15">
@@ -2635,7 +2561,6 @@
         <v>44125</v>
       </c>
       <c r="H20" s="14">
-        <f t="shared" si="0"/>
         <v>47</v>
       </c>
       <c r="I20" s="15">
@@ -2675,7 +2600,6 @@
         <v>674</v>
       </c>
       <c r="U20" s="16">
-        <f t="shared" si="1"/>
         <v>46.25</v>
       </c>
       <c r="V20" s="15">
@@ -2685,7 +2609,6 @@
         <v>44.5</v>
       </c>
       <c r="X20" s="16">
-        <f t="shared" si="2"/>
         <v>51.55</v>
       </c>
       <c r="Y20" s="15">
@@ -2695,7 +2618,6 @@
         <v>49.6</v>
       </c>
       <c r="AA20" s="16">
-        <f t="shared" si="3"/>
         <v>-5.8000000000000007</v>
       </c>
       <c r="AB20" s="15">
@@ -2728,7 +2650,6 @@
         <v>44082</v>
       </c>
       <c r="H21" s="14">
-        <f t="shared" si="0"/>
         <v>73</v>
       </c>
       <c r="I21" s="15">
@@ -2768,7 +2689,6 @@
         <v>655</v>
       </c>
       <c r="U21" s="16">
-        <f t="shared" si="1"/>
         <v>41.2</v>
       </c>
       <c r="V21" s="15">
@@ -2778,7 +2698,6 @@
         <v>40.700000000000003</v>
       </c>
       <c r="X21" s="16">
-        <f t="shared" si="2"/>
         <v>45.849999999999994</v>
       </c>
       <c r="Y21" s="15">
@@ -2788,7 +2707,6 @@
         <v>45.3</v>
       </c>
       <c r="AA21" s="16">
-        <f t="shared" si="3"/>
         <v>-5.2</v>
       </c>
       <c r="AB21" s="15">
@@ -2821,7 +2739,6 @@
         <v>45056</v>
       </c>
       <c r="H22" s="14">
-        <f t="shared" si="0"/>
         <v>70</v>
       </c>
       <c r="I22" s="15">
@@ -2861,7 +2778,6 @@
         <v>578</v>
       </c>
       <c r="U22" s="16">
-        <f t="shared" si="1"/>
         <v>39.700000000000003</v>
       </c>
       <c r="V22" s="15">
@@ -2871,7 +2787,6 @@
         <v>38.6</v>
       </c>
       <c r="X22" s="16">
-        <f t="shared" si="2"/>
         <v>44.2</v>
       </c>
       <c r="Y22" s="15">
@@ -2881,7 +2796,6 @@
         <v>43</v>
       </c>
       <c r="AA22" s="16">
-        <f t="shared" si="3"/>
         <v>-5.4</v>
       </c>
       <c r="AB22" s="15">
@@ -2914,7 +2828,6 @@
         <v>45364</v>
       </c>
       <c r="H23" s="14">
-        <f t="shared" si="0"/>
         <v>58</v>
       </c>
       <c r="I23" s="15">
@@ -2954,7 +2867,6 @@
         <v>644</v>
       </c>
       <c r="U23" s="16">
-        <f t="shared" si="1"/>
         <v>44.4</v>
       </c>
       <c r="V23" s="15">
@@ -2964,7 +2876,6 @@
         <v>43.8</v>
       </c>
       <c r="X23" s="16">
-        <f t="shared" si="2"/>
         <v>49.45</v>
       </c>
       <c r="Y23" s="15">
@@ -2974,7 +2885,6 @@
         <v>48.8</v>
       </c>
       <c r="AA23" s="16">
-        <f t="shared" si="3"/>
         <v>-6.3</v>
       </c>
       <c r="AB23" s="15">
@@ -3007,7 +2917,6 @@
         <v>43439</v>
       </c>
       <c r="H24" s="14">
-        <f t="shared" si="0"/>
         <v>61</v>
       </c>
       <c r="I24" s="15">
@@ -3047,7 +2956,6 @@
         <v>622</v>
       </c>
       <c r="U24" s="16">
-        <f t="shared" si="1"/>
         <v>42.45</v>
       </c>
       <c r="V24" s="15">
@@ -3057,7 +2965,6 @@
         <v>41.8</v>
       </c>
       <c r="X24" s="16">
-        <f t="shared" si="2"/>
         <v>47.3</v>
       </c>
       <c r="Y24" s="15">
@@ -3067,7 +2974,6 @@
         <v>46.5</v>
       </c>
       <c r="AA24" s="16">
-        <f t="shared" si="3"/>
         <v>-5.1999999999999993</v>
       </c>
       <c r="AB24" s="15">
@@ -3100,7 +3006,6 @@
         <v>45245</v>
       </c>
       <c r="H25" s="14">
-        <f t="shared" si="0"/>
         <v>66</v>
       </c>
       <c r="I25" s="15">
@@ -3140,7 +3045,6 @@
         <v>565</v>
       </c>
       <c r="U25" s="16">
-        <f t="shared" si="1"/>
         <v>46.15</v>
       </c>
       <c r="V25" s="15">
@@ -3150,7 +3054,6 @@
         <v>45.4</v>
       </c>
       <c r="X25" s="16">
-        <f t="shared" si="2"/>
         <v>51.45</v>
       </c>
       <c r="Y25" s="15">
@@ -3160,7 +3063,6 @@
         <v>50.6</v>
       </c>
       <c r="AA25" s="16">
-        <f t="shared" si="3"/>
         <v>-6.3</v>
       </c>
       <c r="AB25" s="15">
@@ -3193,7 +3095,6 @@
         <v>44755</v>
       </c>
       <c r="H26" s="14">
-        <f t="shared" si="0"/>
         <v>63</v>
       </c>
       <c r="I26" s="15">
@@ -3233,7 +3134,6 @@
         <v>448</v>
       </c>
       <c r="U26" s="16">
-        <f t="shared" si="1"/>
         <v>40.299999999999997</v>
       </c>
       <c r="V26" s="15">
@@ -3243,7 +3143,6 @@
         <v>39.4</v>
       </c>
       <c r="X26" s="16">
-        <f t="shared" si="2"/>
         <v>44.9</v>
       </c>
       <c r="Y26" s="15">
@@ -3253,7 +3152,6 @@
         <v>43.9</v>
       </c>
       <c r="AA26" s="16">
-        <f t="shared" si="3"/>
         <v>-6.25</v>
       </c>
       <c r="AB26" s="15">
@@ -3286,7 +3184,6 @@
         <v>43859</v>
       </c>
       <c r="H27" s="14">
-        <f t="shared" si="0"/>
         <v>71</v>
       </c>
       <c r="I27" s="15">
@@ -3326,7 +3223,6 @@
         <v>656</v>
       </c>
       <c r="U27" s="16">
-        <f t="shared" si="1"/>
         <v>45.15</v>
       </c>
       <c r="V27" s="15">
@@ -3336,7 +3232,6 @@
         <v>44.9</v>
       </c>
       <c r="X27" s="16">
-        <f t="shared" si="2"/>
         <v>50.3</v>
       </c>
       <c r="Y27" s="15">
@@ -3346,7 +3241,6 @@
         <v>50</v>
       </c>
       <c r="AA27" s="16">
-        <f t="shared" si="3"/>
         <v>-5.9</v>
       </c>
       <c r="AB27" s="15">
@@ -3379,7 +3273,6 @@
         <v>44944</v>
       </c>
       <c r="H28" s="14">
-        <f t="shared" si="0"/>
         <v>56</v>
       </c>
       <c r="I28" s="15">
@@ -3419,7 +3312,6 @@
         <v>623</v>
       </c>
       <c r="U28" s="16">
-        <f t="shared" si="1"/>
         <v>39.049999999999997</v>
       </c>
       <c r="V28" s="15">
@@ -3429,7 +3321,6 @@
         <v>38.700000000000003</v>
       </c>
       <c r="X28" s="16">
-        <f t="shared" si="2"/>
         <v>43.55</v>
       </c>
       <c r="Y28" s="15">
@@ -3439,7 +3330,6 @@
         <v>43.2</v>
       </c>
       <c r="AA28" s="16">
-        <f t="shared" si="3"/>
         <v>-5.35</v>
       </c>
       <c r="AB28" s="15">
@@ -3472,7 +3362,6 @@
         <v>45253</v>
       </c>
       <c r="H29" s="14">
-        <f t="shared" si="0"/>
         <v>57</v>
       </c>
       <c r="I29" s="15">
@@ -3512,7 +3401,6 @@
         <v>654</v>
       </c>
       <c r="U29" s="16">
-        <f t="shared" si="1"/>
         <v>39.6</v>
       </c>
       <c r="V29" s="15">
@@ -3522,7 +3410,6 @@
         <v>39</v>
       </c>
       <c r="X29" s="16">
-        <f t="shared" si="2"/>
         <v>44.15</v>
       </c>
       <c r="Y29" s="15">
@@ -3532,7 +3419,6 @@
         <v>43.5</v>
       </c>
       <c r="AA29" s="16">
-        <f t="shared" si="3"/>
         <v>-5.25</v>
       </c>
       <c r="AB29" s="15">
@@ -3565,7 +3451,6 @@
         <v>45056</v>
       </c>
       <c r="H30" s="14">
-        <f t="shared" si="0"/>
         <v>73</v>
       </c>
       <c r="I30" s="15">
@@ -3605,7 +3490,6 @@
         <v>665</v>
       </c>
       <c r="U30" s="16">
-        <f t="shared" si="1"/>
         <v>44.65</v>
       </c>
       <c r="V30" s="15">
@@ -3615,7 +3499,6 @@
         <v>44.5</v>
       </c>
       <c r="X30" s="16">
-        <f t="shared" si="2"/>
         <v>49.7</v>
       </c>
       <c r="Y30" s="15">
@@ -3625,7 +3508,6 @@
         <v>49.5</v>
       </c>
       <c r="AA30" s="16">
-        <f t="shared" si="3"/>
         <v>-5.9</v>
       </c>
       <c r="AB30" s="15">
@@ -3658,7 +3540,6 @@
         <v>44510</v>
       </c>
       <c r="H31" s="14">
-        <f t="shared" si="0"/>
         <v>79</v>
       </c>
       <c r="I31" s="15">
@@ -3698,7 +3579,6 @@
         <v>585</v>
       </c>
       <c r="U31" s="16">
-        <f t="shared" si="1"/>
         <v>42.5</v>
       </c>
       <c r="V31" s="15">
@@ -3708,7 +3588,6 @@
         <v>42</v>
       </c>
       <c r="X31" s="16">
-        <f t="shared" si="2"/>
         <v>47.349999999999994</v>
       </c>
       <c r="Y31" s="15">
@@ -3718,7 +3597,6 @@
         <v>46.8</v>
       </c>
       <c r="AA31" s="16">
-        <f t="shared" si="3"/>
         <v>-5.8000000000000007</v>
       </c>
       <c r="AB31" s="15">
@@ -3751,7 +3629,6 @@
         <v>44965</v>
       </c>
       <c r="H32" s="14">
-        <f t="shared" si="0"/>
         <v>64</v>
       </c>
       <c r="I32" s="15">
@@ -3791,7 +3668,6 @@
         <v>525</v>
       </c>
       <c r="U32" s="16">
-        <f t="shared" si="1"/>
         <v>41.349999999999994</v>
       </c>
       <c r="V32" s="15">
@@ -3801,7 +3677,6 @@
         <v>40.799999999999997</v>
       </c>
       <c r="X32" s="16">
-        <f t="shared" si="2"/>
         <v>46.1</v>
       </c>
       <c r="Y32" s="15">
@@ -3811,7 +3686,6 @@
         <v>45.5</v>
       </c>
       <c r="AA32" s="16">
-        <f t="shared" si="3"/>
         <v>-5.75</v>
       </c>
       <c r="AB32" s="15">
@@ -3844,7 +3718,6 @@
         <v>44209</v>
       </c>
       <c r="H33" s="14">
-        <f t="shared" si="0"/>
         <v>61</v>
       </c>
       <c r="I33" s="15">
@@ -3884,7 +3757,6 @@
         <v>589</v>
       </c>
       <c r="U33" s="16">
-        <f t="shared" si="1"/>
         <v>43.85</v>
       </c>
       <c r="V33" s="15">
@@ -3894,7 +3766,6 @@
         <v>43.6</v>
       </c>
       <c r="X33" s="16">
-        <f t="shared" si="2"/>
         <v>48.85</v>
       </c>
       <c r="Y33" s="15">
@@ -3904,7 +3775,6 @@
         <v>48.6</v>
       </c>
       <c r="AA33" s="16">
-        <f t="shared" si="3"/>
         <v>-5.75</v>
       </c>
       <c r="AB33" s="15">
@@ -3937,7 +3807,6 @@
         <v>44004</v>
       </c>
       <c r="H34" s="14">
-        <f t="shared" si="0"/>
         <v>57</v>
       </c>
       <c r="I34" s="15">
@@ -3977,7 +3846,6 @@
         <v>650</v>
       </c>
       <c r="U34" s="16">
-        <f t="shared" si="1"/>
         <v>40.200000000000003</v>
       </c>
       <c r="V34" s="15">
@@ -3987,7 +3855,6 @@
         <v>37.799999999999997</v>
       </c>
       <c r="X34" s="16">
-        <f t="shared" si="2"/>
         <v>44.8</v>
       </c>
       <c r="Y34" s="15">
@@ -3997,7 +3864,6 @@
         <v>42.1</v>
       </c>
       <c r="AA34" s="16">
-        <f t="shared" si="3"/>
         <v>-5.65</v>
       </c>
       <c r="AB34" s="15">
@@ -4030,7 +3896,6 @@
         <v>42830</v>
       </c>
       <c r="H35" s="14">
-        <f t="shared" si="0"/>
         <v>70</v>
       </c>
       <c r="I35" s="15">
@@ -4070,7 +3935,6 @@
         <v>611</v>
       </c>
       <c r="U35" s="16">
-        <f t="shared" si="1"/>
         <v>45.25</v>
       </c>
       <c r="V35" s="15">
@@ -4080,7 +3944,6 @@
         <v>44.9</v>
       </c>
       <c r="X35" s="16">
-        <f t="shared" si="2"/>
         <v>50.4</v>
       </c>
       <c r="Y35" s="15">
@@ -4090,7 +3953,6 @@
         <v>50</v>
       </c>
       <c r="AA35" s="16">
-        <f t="shared" si="3"/>
         <v>-5.75</v>
       </c>
       <c r="AB35" s="15">
@@ -4123,7 +3985,6 @@
         <v>43054</v>
       </c>
       <c r="H36" s="14">
-        <f t="shared" si="0"/>
         <v>75</v>
       </c>
       <c r="I36" s="15">
@@ -4163,7 +4024,6 @@
         <v>544</v>
       </c>
       <c r="U36" s="16">
-        <f t="shared" si="1"/>
         <v>41.8</v>
       </c>
       <c r="V36" s="15">
@@ -4173,7 +4033,6 @@
         <v>41</v>
       </c>
       <c r="X36" s="16">
-        <f t="shared" si="2"/>
         <v>46.95</v>
       </c>
       <c r="Y36" s="15">
@@ -4183,7 +4042,6 @@
         <v>46.4</v>
       </c>
       <c r="AA36" s="16">
-        <f t="shared" si="3"/>
         <v>-5.75</v>
       </c>
       <c r="AB36" s="15">
@@ -4216,7 +4074,6 @@
         <v>44097</v>
       </c>
       <c r="H37" s="14">
-        <f t="shared" si="0"/>
         <v>70</v>
       </c>
       <c r="I37" s="15">
@@ -4256,7 +4113,6 @@
         <v>573</v>
       </c>
       <c r="U37" s="16">
-        <f t="shared" si="1"/>
         <v>44.4</v>
       </c>
       <c r="V37" s="15">
@@ -4266,7 +4122,6 @@
         <v>44.3</v>
       </c>
       <c r="X37" s="16">
-        <f t="shared" si="2"/>
         <v>49.45</v>
       </c>
       <c r="Y37" s="15">
@@ -4276,7 +4131,6 @@
         <v>49.4</v>
       </c>
       <c r="AA37" s="16">
-        <f t="shared" si="3"/>
         <v>-5.8</v>
       </c>
       <c r="AB37" s="15">
@@ -4309,7 +4163,6 @@
         <v>44104</v>
       </c>
       <c r="H38" s="14">
-        <f t="shared" si="0"/>
         <v>52</v>
       </c>
       <c r="I38" s="15">
@@ -4349,7 +4202,6 @@
         <v>628</v>
       </c>
       <c r="U38" s="16">
-        <f t="shared" si="1"/>
         <v>45.05</v>
       </c>
       <c r="V38" s="15">
@@ -4359,7 +4211,6 @@
         <v>44.9</v>
       </c>
       <c r="X38" s="16">
-        <f t="shared" si="2"/>
         <v>50.15</v>
       </c>
       <c r="Y38" s="15">
@@ -4369,7 +4220,6 @@
         <v>50</v>
       </c>
       <c r="AA38" s="16">
-        <f t="shared" si="3"/>
         <v>-5.95</v>
       </c>
       <c r="AB38" s="15">
@@ -4402,7 +4252,6 @@
         <v>44216</v>
       </c>
       <c r="H39" s="14">
-        <f t="shared" si="0"/>
         <v>56</v>
       </c>
       <c r="I39" s="15">
@@ -4442,7 +4291,6 @@
         <v>611</v>
       </c>
       <c r="U39" s="16">
-        <f t="shared" si="1"/>
         <v>44.7</v>
       </c>
       <c r="V39" s="15">
@@ -4452,7 +4300,6 @@
         <v>44.1</v>
       </c>
       <c r="X39" s="16">
-        <f t="shared" si="2"/>
         <v>49.8</v>
       </c>
       <c r="Y39" s="15">
@@ -4462,7 +4309,6 @@
         <v>49.1</v>
       </c>
       <c r="AA39" s="16">
-        <f t="shared" si="3"/>
         <v>-5.85</v>
       </c>
       <c r="AB39" s="15">
@@ -4495,7 +4341,6 @@
         <v>44762</v>
       </c>
       <c r="H40" s="14">
-        <f t="shared" si="0"/>
         <v>57</v>
       </c>
       <c r="I40" s="15">
@@ -4535,7 +4380,6 @@
         <v>559</v>
       </c>
       <c r="U40" s="16">
-        <f t="shared" si="1"/>
         <v>45.2</v>
       </c>
       <c r="V40" s="15">
@@ -4545,7 +4389,6 @@
         <v>44.1</v>
       </c>
       <c r="X40" s="16">
-        <f t="shared" si="2"/>
         <v>50.35</v>
       </c>
       <c r="Y40" s="15">
@@ -4555,7 +4398,6 @@
         <v>49.1</v>
       </c>
       <c r="AA40" s="16">
-        <f t="shared" si="3"/>
         <v>-6.4499999999999993</v>
       </c>
       <c r="AB40" s="15">
@@ -4588,7 +4430,6 @@
         <v>44711</v>
       </c>
       <c r="H41" s="14">
-        <f t="shared" si="0"/>
         <v>55</v>
       </c>
       <c r="I41" s="15">
@@ -4628,7 +4469,6 @@
         <v>595</v>
       </c>
       <c r="U41" s="16">
-        <f t="shared" si="1"/>
         <v>43</v>
       </c>
       <c r="V41" s="15">
@@ -4638,7 +4478,6 @@
         <v>42.8</v>
       </c>
       <c r="X41" s="16">
-        <f t="shared" si="2"/>
         <v>47.900000000000006</v>
       </c>
       <c r="Y41" s="15">
@@ -4648,7 +4487,6 @@
         <v>47.6</v>
       </c>
       <c r="AA41" s="16">
-        <f t="shared" si="3"/>
         <v>-5.65</v>
       </c>
       <c r="AB41" s="15">
@@ -4681,7 +4519,6 @@
         <v>44608</v>
       </c>
       <c r="H42" s="14">
-        <f t="shared" si="0"/>
         <v>59</v>
       </c>
       <c r="I42" s="15">
@@ -4721,7 +4558,6 @@
         <v>592</v>
       </c>
       <c r="U42" s="16">
-        <f t="shared" si="1"/>
         <v>43.7</v>
       </c>
       <c r="V42" s="15">
@@ -4731,7 +4567,6 @@
         <v>42.9</v>
       </c>
       <c r="X42" s="16">
-        <f t="shared" si="2"/>
         <v>48.6</v>
       </c>
       <c r="Y42" s="15">
@@ -4741,7 +4576,6 @@
         <v>47.7</v>
       </c>
       <c r="AA42" s="16">
-        <f t="shared" si="3"/>
         <v>-6.2</v>
       </c>
       <c r="AB42" s="15">
@@ -4774,7 +4608,6 @@
         <v>45259</v>
       </c>
       <c r="H43" s="14">
-        <f t="shared" si="0"/>
         <v>78</v>
       </c>
       <c r="I43" s="15">
@@ -4814,7 +4647,6 @@
         <v>700</v>
       </c>
       <c r="U43" s="16">
-        <f t="shared" si="1"/>
         <v>43.099999999999994</v>
       </c>
       <c r="V43" s="15">
@@ -4824,7 +4656,6 @@
         <v>42.8</v>
       </c>
       <c r="X43" s="16">
-        <f t="shared" si="2"/>
         <v>48</v>
       </c>
       <c r="Y43" s="15">
@@ -4834,7 +4665,6 @@
         <v>47.7</v>
       </c>
       <c r="AA43" s="16">
-        <f t="shared" si="3"/>
         <v>-5.4</v>
       </c>
       <c r="AB43" s="15">
@@ -4867,7 +4697,6 @@
         <v>44013</v>
       </c>
       <c r="H44" s="14">
-        <f t="shared" si="0"/>
         <v>63</v>
       </c>
       <c r="I44" s="15">
@@ -4907,7 +4736,6 @@
         <v>560</v>
       </c>
       <c r="U44" s="16">
-        <f t="shared" si="1"/>
         <v>44.400000000000006</v>
       </c>
       <c r="V44" s="15">
@@ -4917,7 +4745,6 @@
         <v>44.1</v>
       </c>
       <c r="X44" s="16">
-        <f t="shared" si="2"/>
         <v>49.45</v>
       </c>
       <c r="Y44" s="15">
@@ -4927,7 +4754,6 @@
         <v>49.1</v>
       </c>
       <c r="AA44" s="16">
-        <f t="shared" si="3"/>
         <v>-6.05</v>
       </c>
       <c r="AB44" s="15">
@@ -4960,7 +4786,6 @@
         <v>45448</v>
       </c>
       <c r="H45" s="14">
-        <f t="shared" si="0"/>
         <v>60</v>
       </c>
       <c r="I45" s="15">
@@ -5000,7 +4825,6 @@
         <v>630</v>
       </c>
       <c r="U45" s="16">
-        <f t="shared" si="1"/>
         <v>45.349999999999994</v>
       </c>
       <c r="V45" s="15">
@@ -5010,7 +4834,6 @@
         <v>43.9</v>
       </c>
       <c r="X45" s="16">
-        <f t="shared" si="2"/>
         <v>50.55</v>
       </c>
       <c r="Y45" s="15">
@@ -5020,7 +4843,6 @@
         <v>48.9</v>
       </c>
       <c r="AA45" s="16">
-        <f t="shared" si="3"/>
         <v>-6.1999999999999993</v>
       </c>
       <c r="AB45" s="15">
@@ -5053,7 +4875,6 @@
         <v>44251</v>
       </c>
       <c r="H46" s="14">
-        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="I46" s="15">
@@ -5093,7 +4914,6 @@
         <v>783</v>
       </c>
       <c r="U46" s="16">
-        <f t="shared" si="1"/>
         <v>41.65</v>
       </c>
       <c r="V46" s="15">
@@ -5103,7 +4923,6 @@
         <v>41.3</v>
       </c>
       <c r="X46" s="16">
-        <f t="shared" si="2"/>
         <v>46.35</v>
       </c>
       <c r="Y46" s="15">
@@ -5113,7 +4932,6 @@
         <v>46</v>
       </c>
       <c r="AA46" s="16">
-        <f t="shared" si="3"/>
         <v>-6.45</v>
       </c>
       <c r="AB46" s="15">
@@ -5146,7 +4964,6 @@
         <v>43810</v>
       </c>
       <c r="H47" s="14">
-        <f t="shared" si="0"/>
         <v>61</v>
       </c>
       <c r="I47" s="15">
@@ -5186,7 +5003,6 @@
         <v>675</v>
       </c>
       <c r="U47" s="16">
-        <f t="shared" si="1"/>
         <v>41.7</v>
       </c>
       <c r="V47" s="15">
@@ -5196,7 +5012,6 @@
         <v>41.2</v>
       </c>
       <c r="X47" s="16">
-        <f t="shared" si="2"/>
         <v>46.5</v>
       </c>
       <c r="Y47" s="15">
@@ -5206,7 +5021,6 @@
         <v>46</v>
       </c>
       <c r="AA47" s="16">
-        <f t="shared" si="3"/>
         <v>-5.1999999999999993</v>
       </c>
       <c r="AB47" s="15">
@@ -5239,7 +5053,6 @@
         <v>43971</v>
       </c>
       <c r="H48" s="14">
-        <f t="shared" si="0"/>
         <v>61</v>
       </c>
       <c r="I48" s="15">
@@ -5279,7 +5092,6 @@
         <v>608</v>
       </c>
       <c r="U48" s="16">
-        <f t="shared" si="1"/>
         <v>41.35</v>
       </c>
       <c r="V48" s="15">
@@ -5289,7 +5101,6 @@
         <v>41</v>
       </c>
       <c r="X48" s="16">
-        <f t="shared" si="2"/>
         <v>46.05</v>
       </c>
       <c r="Y48" s="15">
@@ -5299,7 +5110,6 @@
         <v>45.6</v>
       </c>
       <c r="AA48" s="16">
-        <f t="shared" si="3"/>
         <v>-5.15</v>
       </c>
       <c r="AB48" s="15">
@@ -5332,7 +5142,6 @@
         <v>44979</v>
       </c>
       <c r="H49" s="14">
-        <f t="shared" si="0"/>
         <v>64</v>
       </c>
       <c r="I49" s="15">
@@ -5372,7 +5181,6 @@
         <v>523</v>
       </c>
       <c r="U49" s="16">
-        <f t="shared" si="1"/>
         <v>45.05</v>
       </c>
       <c r="V49" s="15">
@@ -5382,7 +5190,6 @@
         <v>44.3</v>
       </c>
       <c r="X49" s="16">
-        <f t="shared" si="2"/>
         <v>50.2</v>
       </c>
       <c r="Y49" s="15">
@@ -5392,7 +5199,6 @@
         <v>49.3</v>
       </c>
       <c r="AA49" s="16">
-        <f t="shared" si="3"/>
         <v>-6.0500000000000007</v>
       </c>
       <c r="AB49" s="15">
@@ -5425,7 +5231,6 @@
         <v>44125</v>
       </c>
       <c r="H50" s="14">
-        <f t="shared" si="0"/>
         <v>68</v>
       </c>
       <c r="I50" s="15">
@@ -5465,7 +5270,6 @@
         <v>657</v>
       </c>
       <c r="U50" s="16">
-        <f t="shared" si="1"/>
         <v>44.05</v>
       </c>
       <c r="V50" s="15">
@@ -5475,7 +5279,6 @@
         <v>43.9</v>
       </c>
       <c r="X50" s="16">
-        <f t="shared" si="2"/>
         <v>49.05</v>
       </c>
       <c r="Y50" s="15">
@@ -5485,7 +5288,6 @@
         <v>48.9</v>
       </c>
       <c r="AA50" s="16">
-        <f t="shared" si="3"/>
         <v>-5.3000000000000007</v>
       </c>
       <c r="AB50" s="15">
@@ -5518,7 +5320,6 @@
         <v>44251</v>
       </c>
       <c r="H51" s="14">
-        <f t="shared" si="0"/>
         <v>68</v>
       </c>
       <c r="I51" s="15">
@@ -5558,7 +5359,6 @@
         <v>638</v>
       </c>
       <c r="U51" s="16">
-        <f t="shared" si="1"/>
         <v>44.65</v>
       </c>
       <c r="V51" s="15">
@@ -5568,7 +5368,6 @@
         <v>44.3</v>
       </c>
       <c r="X51" s="16">
-        <f t="shared" si="2"/>
         <v>49.75</v>
       </c>
       <c r="Y51" s="15">
@@ -5578,7 +5377,6 @@
         <v>49.4</v>
       </c>
       <c r="AA51" s="16">
-        <f t="shared" si="3"/>
         <v>-5.6</v>
       </c>
       <c r="AB51" s="15">
@@ -5611,7 +5409,6 @@
         <v>44952</v>
       </c>
       <c r="H52" s="14">
-        <f t="shared" si="0"/>
         <v>70</v>
       </c>
       <c r="I52" s="15">
@@ -5651,7 +5448,6 @@
         <v>678</v>
       </c>
       <c r="U52" s="16">
-        <f t="shared" si="1"/>
         <v>41.15</v>
       </c>
       <c r="V52" s="15">
@@ -5661,7 +5457,6 @@
         <v>40.799999999999997</v>
       </c>
       <c r="X52" s="16">
-        <f t="shared" si="2"/>
         <v>45.9</v>
       </c>
       <c r="Y52" s="15">
@@ -5671,7 +5466,6 @@
         <v>45.5</v>
       </c>
       <c r="AA52" s="16">
-        <f t="shared" si="3"/>
         <v>-5.4499999999999993</v>
       </c>
       <c r="AB52" s="15">
@@ -5704,7 +5498,6 @@
         <v>45595</v>
       </c>
       <c r="H53" s="14">
-        <f t="shared" si="0"/>
         <v>59</v>
       </c>
       <c r="I53" s="15">
@@ -5744,7 +5537,6 @@
         <v>574</v>
       </c>
       <c r="U53" s="16">
-        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="V53" s="15">
@@ -5754,7 +5546,6 @@
         <v>39.200000000000003</v>
       </c>
       <c r="X53" s="16">
-        <f t="shared" si="2"/>
         <v>44.55</v>
       </c>
       <c r="Y53" s="15">
@@ -5764,7 +5555,6 @@
         <v>43.7</v>
       </c>
       <c r="AA53" s="16">
-        <f t="shared" si="3"/>
         <v>-5.4499999999999993</v>
       </c>
       <c r="AB53" s="15">
@@ -5797,7 +5587,6 @@
         <v>44314</v>
       </c>
       <c r="H54" s="14">
-        <f t="shared" si="0"/>
         <v>79</v>
       </c>
       <c r="I54" s="15">
@@ -5837,7 +5626,6 @@
         <v>528</v>
       </c>
       <c r="U54" s="16">
-        <f t="shared" si="1"/>
         <v>44.55</v>
       </c>
       <c r="V54" s="15">
@@ -5847,7 +5635,6 @@
         <v>44.5</v>
       </c>
       <c r="X54" s="16">
-        <f t="shared" si="2"/>
         <v>44.585000000000001</v>
       </c>
       <c r="Y54" s="15">
@@ -5857,7 +5644,6 @@
         <v>44.47</v>
       </c>
       <c r="AA54" s="16">
-        <f t="shared" si="3"/>
         <v>-6</v>
       </c>
       <c r="AB54" s="15">
@@ -5890,7 +5676,6 @@
         <v>44363</v>
       </c>
       <c r="H55" s="14">
-        <f t="shared" si="0"/>
         <v>66</v>
       </c>
       <c r="I55" s="15">
@@ -5930,7 +5715,6 @@
         <v>563</v>
       </c>
       <c r="U55" s="16">
-        <f t="shared" si="1"/>
         <v>46.5</v>
       </c>
       <c r="V55" s="15">
@@ -5940,7 +5724,6 @@
         <v>46.2</v>
       </c>
       <c r="X55" s="16">
-        <f t="shared" si="2"/>
         <v>51.85</v>
       </c>
       <c r="Y55" s="15">
@@ -5950,7 +5733,6 @@
         <v>51.5</v>
       </c>
       <c r="AA55" s="16">
-        <f t="shared" si="3"/>
         <v>-6.4</v>
       </c>
       <c r="AB55" s="15">
@@ -5983,7 +5765,6 @@
         <v>45378</v>
       </c>
       <c r="H56" s="14">
-        <f t="shared" si="0"/>
         <v>66</v>
       </c>
       <c r="I56" s="15">
@@ -6011,7 +5792,6 @@
         <v>4.05</v>
       </c>
       <c r="Q56" s="15">
-        <f>T56</f>
         <v>577</v>
       </c>
       <c r="R56" s="15">
@@ -6024,7 +5804,6 @@
         <v>577</v>
       </c>
       <c r="U56" s="16">
-        <f t="shared" si="1"/>
         <v>45.45</v>
       </c>
       <c r="V56" s="15">
@@ -6034,7 +5813,6 @@
         <v>45.1</v>
       </c>
       <c r="X56" s="16">
-        <f t="shared" si="2"/>
         <v>50.65</v>
       </c>
       <c r="Y56" s="15">
@@ -6044,7 +5822,6 @@
         <v>50.3</v>
       </c>
       <c r="AA56" s="16">
-        <f t="shared" si="3"/>
         <v>-6.3</v>
       </c>
       <c r="AB56" s="15">
@@ -6077,7 +5854,6 @@
         <v>44734</v>
       </c>
       <c r="H57" s="14">
-        <f t="shared" si="0"/>
         <v>61</v>
       </c>
       <c r="I57" s="15">
@@ -6117,7 +5893,6 @@
         <v>655</v>
       </c>
       <c r="U57" s="16">
-        <f t="shared" si="1"/>
         <v>40.299999999999997</v>
       </c>
       <c r="V57" s="15">
@@ -6127,7 +5902,6 @@
         <v>40.1</v>
       </c>
       <c r="X57" s="16">
-        <f t="shared" si="2"/>
         <v>44.900000000000006</v>
       </c>
       <c r="Y57" s="15">
@@ -6137,7 +5911,6 @@
         <v>44.7</v>
       </c>
       <c r="AA57" s="16">
-        <f t="shared" si="3"/>
         <v>-5.25</v>
       </c>
       <c r="AB57" s="15">
@@ -6170,7 +5943,6 @@
         <v>44244</v>
       </c>
       <c r="H58" s="14">
-        <f t="shared" si="0"/>
         <v>64</v>
       </c>
       <c r="I58" s="15">
@@ -6210,7 +5982,6 @@
         <v>624</v>
       </c>
       <c r="U58" s="16">
-        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="V58" s="15">
@@ -6220,7 +5991,6 @@
         <v>44.7</v>
       </c>
       <c r="X58" s="16">
-        <f t="shared" si="2"/>
         <v>50.15</v>
       </c>
       <c r="Y58" s="15">
@@ -6230,7 +6000,6 @@
         <v>49.8</v>
       </c>
       <c r="AA58" s="16">
-        <f t="shared" si="3"/>
         <v>-5.65</v>
       </c>
       <c r="AB58" s="15">
@@ -6263,7 +6032,6 @@
         <v>43991</v>
       </c>
       <c r="H59" s="14">
-        <f t="shared" si="0"/>
         <v>72</v>
       </c>
       <c r="I59" s="15">
@@ -6291,7 +6059,6 @@
         <v>4.83</v>
       </c>
       <c r="Q59" s="15">
-        <f>T59</f>
         <v>873</v>
       </c>
       <c r="R59" s="15">
@@ -6304,7 +6071,6 @@
         <v>873</v>
       </c>
       <c r="U59" s="16">
-        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="V59" s="15">
@@ -6314,7 +6080,6 @@
         <v>43.7</v>
       </c>
       <c r="X59" s="16">
-        <f t="shared" si="2"/>
         <v>50.150000000000006</v>
       </c>
       <c r="Y59" s="15">
@@ -6324,7 +6089,6 @@
         <v>48.7</v>
       </c>
       <c r="AA59" s="16">
-        <f t="shared" si="3"/>
         <v>-5.6999999999999993</v>
       </c>
       <c r="AB59" s="15">
@@ -6357,7 +6121,6 @@
         <v>44601</v>
       </c>
       <c r="H60" s="14">
-        <f t="shared" si="0"/>
         <v>79</v>
       </c>
       <c r="I60" s="15">
@@ -6397,7 +6160,6 @@
         <v>615</v>
       </c>
       <c r="U60" s="16">
-        <f t="shared" si="1"/>
         <v>42.75</v>
       </c>
       <c r="V60" s="15">
@@ -6407,7 +6169,6 @@
         <v>42.6</v>
       </c>
       <c r="X60" s="16">
-        <f t="shared" si="2"/>
         <v>47.65</v>
       </c>
       <c r="Y60" s="15">
@@ -6417,7 +6178,6 @@
         <v>47.5</v>
       </c>
       <c r="AA60" s="16">
-        <f t="shared" si="3"/>
         <v>-6.1</v>
       </c>
       <c r="AB60" s="15">
@@ -6450,7 +6210,6 @@
         <v>44237</v>
       </c>
       <c r="H61" s="14">
-        <f t="shared" si="0"/>
         <v>68</v>
       </c>
       <c r="I61" s="15">
@@ -6490,7 +6249,6 @@
         <v>678</v>
       </c>
       <c r="U61" s="16">
-        <f t="shared" si="1"/>
         <v>43.95</v>
       </c>
       <c r="V61" s="15">
@@ -6500,7 +6258,6 @@
         <v>43.9</v>
       </c>
       <c r="X61" s="16">
-        <f t="shared" si="2"/>
         <v>49</v>
       </c>
       <c r="Y61" s="15">
@@ -6510,7 +6267,6 @@
         <v>48.9</v>
       </c>
       <c r="AA61" s="16">
-        <f t="shared" si="3"/>
         <v>-5.0999999999999996</v>
       </c>
       <c r="AB61" s="15">
@@ -6543,7 +6299,6 @@
         <v>43859</v>
       </c>
       <c r="H62" s="14">
-        <f t="shared" si="0"/>
         <v>75</v>
       </c>
       <c r="I62" s="15">
@@ -6583,7 +6338,6 @@
         <v>586</v>
       </c>
       <c r="U62" s="16">
-        <f t="shared" si="1"/>
         <v>43.400000000000006</v>
       </c>
       <c r="V62" s="15">
@@ -6593,7 +6347,6 @@
         <v>42.6</v>
       </c>
       <c r="X62" s="16">
-        <f t="shared" si="2"/>
         <v>48.349999999999994</v>
       </c>
       <c r="Y62" s="15">
@@ -6603,7 +6356,6 @@
         <v>47.4</v>
       </c>
       <c r="AA62" s="16">
-        <f t="shared" si="3"/>
         <v>-5.6</v>
       </c>
       <c r="AB62" s="15">
@@ -6636,7 +6388,6 @@
         <v>44727</v>
       </c>
       <c r="H63" s="14">
-        <f t="shared" si="0"/>
         <v>71</v>
       </c>
       <c r="I63" s="15">
@@ -6676,7 +6427,6 @@
         <v>611</v>
       </c>
       <c r="U63" s="16">
-        <f t="shared" si="1"/>
         <v>43.6</v>
       </c>
       <c r="V63" s="15">
@@ -6686,7 +6436,6 @@
         <v>43.2</v>
       </c>
       <c r="X63" s="16">
-        <f t="shared" si="2"/>
         <v>48.6</v>
       </c>
       <c r="Y63" s="15">
@@ -6696,7 +6445,6 @@
         <v>48.2</v>
       </c>
       <c r="AA63" s="16">
-        <f t="shared" si="3"/>
         <v>-5.55</v>
       </c>
       <c r="AB63" s="15">
@@ -6729,7 +6477,6 @@
         <v>44327</v>
       </c>
       <c r="H64" s="14">
-        <f t="shared" si="0"/>
         <v>58</v>
       </c>
       <c r="I64" s="15">
@@ -6769,7 +6516,6 @@
         <v>605</v>
       </c>
       <c r="U64" s="16">
-        <f t="shared" si="1"/>
         <v>43.5</v>
       </c>
       <c r="V64" s="15">
@@ -6779,7 +6525,6 @@
         <v>43.2</v>
       </c>
       <c r="X64" s="16">
-        <f t="shared" si="2"/>
         <v>48.45</v>
       </c>
       <c r="Y64" s="15">
@@ -6789,7 +6534,6 @@
         <v>48.1</v>
       </c>
       <c r="AA64" s="16">
-        <f t="shared" si="3"/>
         <v>-5.75</v>
       </c>
       <c r="AB64" s="15">
@@ -6822,7 +6566,6 @@
         <v>44503</v>
       </c>
       <c r="H65" s="14">
-        <f t="shared" si="0"/>
         <v>59</v>
       </c>
       <c r="I65" s="15">
@@ -6862,7 +6605,6 @@
         <v>600</v>
       </c>
       <c r="U65" s="16">
-        <f t="shared" si="1"/>
         <v>43.400000000000006</v>
       </c>
       <c r="V65" s="15">
@@ -6872,7 +6614,6 @@
         <v>43.1</v>
       </c>
       <c r="X65" s="16">
-        <f t="shared" si="2"/>
         <v>48.35</v>
       </c>
       <c r="Y65" s="15">
@@ -6882,7 +6623,6 @@
         <v>48</v>
       </c>
       <c r="AA65" s="16">
-        <f t="shared" si="3"/>
         <v>-5.9</v>
       </c>
       <c r="AB65" s="15">
@@ -6915,7 +6655,6 @@
         <v>44461</v>
       </c>
       <c r="H66" s="14">
-        <f t="shared" si="0"/>
         <v>65</v>
       </c>
       <c r="I66" s="15">
@@ -6955,7 +6694,6 @@
         <v>568</v>
       </c>
       <c r="U66" s="16">
-        <f t="shared" si="1"/>
         <v>42.25</v>
       </c>
       <c r="V66" s="15">
@@ -6965,7 +6703,6 @@
         <v>42.2</v>
       </c>
       <c r="X66" s="16">
-        <f t="shared" si="2"/>
         <v>47.1</v>
       </c>
       <c r="Y66" s="15">
@@ -6975,7 +6712,6 @@
         <v>47</v>
       </c>
       <c r="AA66" s="16">
-        <f t="shared" si="3"/>
         <v>-5.65</v>
       </c>
       <c r="AB66" s="15">
@@ -7008,7 +6744,6 @@
         <v>44720</v>
       </c>
       <c r="H67" s="14">
-        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="I67" s="15">
@@ -7036,7 +6771,6 @@
         <v>3.97</v>
       </c>
       <c r="Q67" s="15">
-        <f>T67</f>
         <v>679</v>
       </c>
       <c r="R67" s="15">
@@ -7049,7 +6783,6 @@
         <v>679</v>
       </c>
       <c r="U67" s="16">
-        <f t="shared" si="1"/>
         <v>43.6</v>
       </c>
       <c r="V67" s="15">
@@ -7059,7 +6792,6 @@
         <v>42</v>
       </c>
       <c r="X67" s="16">
-        <f t="shared" si="2"/>
         <v>48.599999999999994</v>
       </c>
       <c r="Y67" s="15">
@@ -7069,7 +6801,6 @@
         <v>46.8</v>
       </c>
       <c r="AA67" s="16">
-        <f t="shared" si="3"/>
         <v>-5.5</v>
       </c>
       <c r="AB67" s="15">
@@ -7102,7 +6833,6 @@
         <v>44763</v>
       </c>
       <c r="H68" s="14">
-        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="I68" s="15">
@@ -7130,7 +6860,6 @@
         <v>3.88</v>
       </c>
       <c r="Q68" s="15">
-        <f>T68</f>
         <v>686</v>
       </c>
       <c r="R68" s="15">
@@ -7143,7 +6872,6 @@
         <v>686</v>
       </c>
       <c r="U68" s="16">
-        <f t="shared" si="1"/>
         <v>43.85</v>
       </c>
       <c r="V68" s="15">
@@ -7153,7 +6881,6 @@
         <v>42.1</v>
       </c>
       <c r="X68" s="16">
-        <f t="shared" si="2"/>
         <v>48.849999999999994</v>
       </c>
       <c r="Y68" s="15">
@@ -7163,7 +6890,6 @@
         <v>46.9</v>
       </c>
       <c r="AA68" s="16">
-        <f t="shared" si="3"/>
         <v>-5.45</v>
       </c>
       <c r="AB68" s="15">
@@ -7196,7 +6922,6 @@
         <v>44489</v>
       </c>
       <c r="H69" s="14">
-        <f t="shared" si="0"/>
         <v>66</v>
       </c>
       <c r="I69" s="15">
@@ -7236,7 +6961,6 @@
         <v>643</v>
       </c>
       <c r="U69" s="16">
-        <f t="shared" si="1"/>
         <v>43.65</v>
       </c>
       <c r="V69" s="15">
@@ -7246,7 +6970,6 @@
         <v>42.3</v>
       </c>
       <c r="X69" s="16">
-        <f t="shared" si="2"/>
         <v>48.650000000000006</v>
       </c>
       <c r="Y69" s="15">
@@ -7256,7 +6979,6 @@
         <v>47.1</v>
       </c>
       <c r="AA69" s="16">
-        <f t="shared" si="3"/>
         <v>-5.5500000000000007</v>
       </c>
       <c r="AB69" s="15">
@@ -7289,7 +7011,6 @@
         <v>44881</v>
       </c>
       <c r="H70" s="14">
-        <f t="shared" si="0"/>
         <v>79</v>
       </c>
       <c r="I70" s="15">
@@ -7317,7 +7038,6 @@
         <v>4.84</v>
       </c>
       <c r="Q70" s="15">
-        <f>T70</f>
         <v>592</v>
       </c>
       <c r="R70" s="15">
@@ -7330,7 +7050,6 @@
         <v>592</v>
       </c>
       <c r="U70" s="16">
-        <f t="shared" si="1"/>
         <v>46.05</v>
       </c>
       <c r="V70" s="15">
@@ -7340,7 +7059,6 @@
         <v>45.2</v>
       </c>
       <c r="X70" s="16">
-        <f t="shared" si="2"/>
         <v>51.349999999999994</v>
       </c>
       <c r="Y70" s="15">
@@ -7350,7 +7068,6 @@
         <v>50.4</v>
       </c>
       <c r="AA70" s="16">
-        <f t="shared" si="3"/>
         <v>-6.3</v>
       </c>
       <c r="AB70" s="15">
@@ -7383,7 +7100,6 @@
         <v>43416</v>
       </c>
       <c r="H71" s="14">
-        <f t="shared" si="0"/>
         <v>64</v>
       </c>
       <c r="I71" s="15">
@@ -7423,7 +7139,6 @@
         <v>546</v>
       </c>
       <c r="U71" s="16">
-        <f t="shared" si="1"/>
         <v>43.65</v>
       </c>
       <c r="V71" s="15">
@@ -7433,7 +7148,6 @@
         <v>43.4</v>
       </c>
       <c r="X71" s="16">
-        <f t="shared" si="2"/>
         <v>48.599999999999994</v>
       </c>
       <c r="Y71" s="15">
@@ -7443,7 +7157,6 @@
         <v>48.3</v>
       </c>
       <c r="AA71" s="16">
-        <f t="shared" si="3"/>
         <v>-6</v>
       </c>
       <c r="AB71" s="15">
@@ -7476,7 +7189,6 @@
         <v>43775</v>
       </c>
       <c r="H72" s="14">
-        <f t="shared" si="0"/>
         <v>65</v>
       </c>
       <c r="I72" s="15">
@@ -7516,7 +7228,6 @@
         <v>548</v>
       </c>
       <c r="U72" s="16">
-        <f t="shared" si="1"/>
         <v>43.85</v>
       </c>
       <c r="V72" s="15">
@@ -7526,7 +7237,6 @@
         <v>43.6</v>
       </c>
       <c r="X72" s="16">
-        <f t="shared" si="2"/>
         <v>48.8</v>
       </c>
       <c r="Y72" s="15">
@@ -7536,7 +7246,6 @@
         <v>48.5</v>
       </c>
       <c r="AA72" s="16">
-        <f t="shared" si="3"/>
         <v>-6.05</v>
       </c>
       <c r="AB72" s="15">
@@ -7569,7 +7278,6 @@
         <v>44279</v>
       </c>
       <c r="H73" s="14">
-        <f t="shared" si="0"/>
         <v>73</v>
       </c>
       <c r="I73" s="15">
@@ -7609,7 +7317,6 @@
         <v>606</v>
       </c>
       <c r="U73" s="16">
-        <f t="shared" si="1"/>
         <v>41.7</v>
       </c>
       <c r="V73" s="15">
@@ -7619,7 +7326,6 @@
         <v>41.1</v>
       </c>
       <c r="X73" s="16">
-        <f t="shared" si="2"/>
         <v>46.45</v>
       </c>
       <c r="Y73" s="15">
@@ -7629,7 +7335,6 @@
         <v>45.8</v>
       </c>
       <c r="AA73" s="16">
-        <f t="shared" si="3"/>
         <v>-5.5500000000000007</v>
       </c>
       <c r="AB73" s="15">
@@ -7662,7 +7367,6 @@
         <v>45602</v>
       </c>
       <c r="H74" s="14">
-        <f t="shared" si="0"/>
         <v>51</v>
       </c>
       <c r="I74" s="15">
@@ -7702,7 +7406,6 @@
         <v>549</v>
       </c>
       <c r="U74" s="16">
-        <f t="shared" si="1"/>
         <v>47.349999999999994</v>
       </c>
       <c r="V74" s="15">
@@ -7712,7 +7415,6 @@
         <v>46.4</v>
       </c>
       <c r="X74" s="16">
-        <f t="shared" si="2"/>
         <v>52.75</v>
       </c>
       <c r="Y74" s="15">
@@ -7722,7 +7424,6 @@
         <v>51.7</v>
       </c>
       <c r="AA74" s="16">
-        <f t="shared" si="3"/>
         <v>-6.5</v>
       </c>
       <c r="AB74" s="15">
@@ -7755,7 +7456,6 @@
         <v>43710</v>
       </c>
       <c r="H75" s="14">
-        <f t="shared" si="0"/>
         <v>77</v>
       </c>
       <c r="I75" s="15">
@@ -7795,7 +7495,6 @@
         <v>584</v>
       </c>
       <c r="U75" s="16">
-        <f t="shared" si="1"/>
         <v>41.85</v>
       </c>
       <c r="V75" s="15">
@@ -7805,7 +7504,6 @@
         <v>41.5</v>
       </c>
       <c r="X75" s="16">
-        <f t="shared" si="2"/>
         <v>46.6</v>
       </c>
       <c r="Y75" s="15">
@@ -7815,7 +7513,6 @@
         <v>46.2</v>
       </c>
       <c r="AA75" s="16">
-        <f t="shared" si="3"/>
         <v>-5.8000000000000007</v>
       </c>
       <c r="AB75" s="15">
@@ -7848,7 +7545,6 @@
         <v>44895</v>
       </c>
       <c r="H76" s="14">
-        <f t="shared" si="0"/>
         <v>74</v>
       </c>
       <c r="I76" s="15">
@@ -7876,7 +7572,6 @@
         <v>4.58</v>
       </c>
       <c r="Q76" s="15">
-        <f>T76</f>
         <v>673</v>
       </c>
       <c r="R76" s="15">
@@ -7889,7 +7584,6 @@
         <v>673</v>
       </c>
       <c r="U76" s="16">
-        <f t="shared" si="1"/>
         <v>44.150000000000006</v>
       </c>
       <c r="V76" s="15">
@@ -7899,7 +7593,6 @@
         <v>43.7</v>
       </c>
       <c r="X76" s="16">
-        <f t="shared" si="2"/>
         <v>49.150000000000006</v>
       </c>
       <c r="Y76" s="15">
@@ -7909,7 +7602,6 @@
         <v>48.6</v>
       </c>
       <c r="AA76" s="16">
-        <f t="shared" si="3"/>
         <v>-5.6</v>
       </c>
       <c r="AB76" s="15">
@@ -7942,7 +7634,6 @@
         <v>44601</v>
       </c>
       <c r="H77" s="14">
-        <f t="shared" si="0"/>
         <v>67</v>
       </c>
       <c r="I77" s="15">
@@ -7970,7 +7661,6 @@
         <v>4.3899999999999997</v>
       </c>
       <c r="Q77" s="15">
-        <f>T77</f>
         <v>797</v>
       </c>
       <c r="R77" s="15">
@@ -7983,7 +7673,6 @@
         <v>797</v>
       </c>
       <c r="U77" s="16">
-        <f t="shared" si="1"/>
         <v>44.1</v>
       </c>
       <c r="V77" s="15">
@@ -7993,7 +7682,6 @@
         <v>43.2</v>
       </c>
       <c r="X77" s="16">
-        <f t="shared" si="2"/>
         <v>49.1</v>
       </c>
       <c r="Y77" s="15">
@@ -8003,7 +7691,6 @@
         <v>48.1</v>
       </c>
       <c r="AA77" s="16">
-        <f t="shared" si="3"/>
         <v>-6.7</v>
       </c>
       <c r="AB77" s="15">
@@ -8036,7 +7723,6 @@
         <v>43551</v>
       </c>
       <c r="H78" s="14">
-        <f t="shared" si="0"/>
         <v>72</v>
       </c>
       <c r="I78" s="15">
@@ -8076,7 +7762,6 @@
         <v>744</v>
       </c>
       <c r="U78" s="16">
-        <f t="shared" si="1"/>
         <v>43.65</v>
       </c>
       <c r="V78" s="15">
@@ -8086,7 +7771,6 @@
         <v>43.3</v>
       </c>
       <c r="X78" s="16">
-        <f t="shared" si="2"/>
         <v>48.6</v>
       </c>
       <c r="Y78" s="15">
@@ -8096,7 +7780,6 @@
         <v>48.2</v>
       </c>
       <c r="AA78" s="16">
-        <f t="shared" si="3"/>
         <v>-5.6</v>
       </c>
       <c r="AB78" s="15">
@@ -8129,7 +7812,6 @@
         <v>43733</v>
       </c>
       <c r="H79" s="14">
-        <f t="shared" si="0"/>
         <v>73</v>
       </c>
       <c r="I79" s="15">
@@ -8169,7 +7851,6 @@
         <v>696</v>
       </c>
       <c r="U79" s="16">
-        <f t="shared" si="1"/>
         <v>42.95</v>
       </c>
       <c r="V79" s="15">
@@ -8179,7 +7860,6 @@
         <v>42.7</v>
       </c>
       <c r="X79" s="16">
-        <f t="shared" si="2"/>
         <v>47.85</v>
       </c>
       <c r="Y79" s="15">
@@ -8189,7 +7869,6 @@
         <v>47.5</v>
       </c>
       <c r="AA79" s="16">
-        <f t="shared" si="3"/>
         <v>-5.6999999999999993</v>
       </c>
       <c r="AB79" s="15">
@@ -8222,7 +7901,6 @@
         <v>44706</v>
       </c>
       <c r="H80" s="14">
-        <f t="shared" si="0"/>
         <v>68</v>
       </c>
       <c r="I80" s="15">
@@ -8250,7 +7928,6 @@
         <v>5.05</v>
       </c>
       <c r="Q80" s="15">
-        <f>T80</f>
         <v>724</v>
       </c>
       <c r="R80" s="15">
@@ -8263,7 +7940,6 @@
         <v>724</v>
       </c>
       <c r="U80" s="16">
-        <f t="shared" si="1"/>
         <v>43.55</v>
       </c>
       <c r="V80" s="15">
@@ -8273,7 +7949,6 @@
         <v>43.1</v>
       </c>
       <c r="X80" s="16">
-        <f t="shared" si="2"/>
         <v>48.55</v>
       </c>
       <c r="Y80" s="15">
@@ -8283,7 +7958,6 @@
         <v>48.1</v>
       </c>
       <c r="AA80" s="16">
-        <f t="shared" si="3"/>
         <v>-5.25</v>
       </c>
       <c r="AB80" s="15">
@@ -8316,7 +7990,6 @@
         <v>44755</v>
       </c>
       <c r="H81" s="14">
-        <f t="shared" si="0"/>
         <v>66</v>
       </c>
       <c r="I81" s="15" t="s">
@@ -8344,7 +8017,6 @@
         <v>4.5599999999999996</v>
       </c>
       <c r="Q81" s="15">
-        <f>T81</f>
         <v>745</v>
       </c>
       <c r="R81" s="15">
@@ -8357,7 +8029,6 @@
         <v>745</v>
       </c>
       <c r="U81" s="16">
-        <f t="shared" si="1"/>
         <v>42</v>
       </c>
       <c r="V81" s="15">
@@ -8367,7 +8038,6 @@
         <v>39</v>
       </c>
       <c r="X81" s="16">
-        <f t="shared" si="2"/>
         <v>46.8</v>
       </c>
       <c r="Y81" s="15">
@@ -8377,7 +8047,6 @@
         <v>43.4</v>
       </c>
       <c r="AA81" s="16">
-        <f t="shared" si="3"/>
         <v>-5.75</v>
       </c>
       <c r="AB81" s="15">
@@ -8410,7 +8079,6 @@
         <v>45252</v>
       </c>
       <c r="H82" s="14">
-        <f t="shared" si="0"/>
         <v>41</v>
       </c>
       <c r="I82" s="15">
@@ -8450,7 +8118,6 @@
         <v>857</v>
       </c>
       <c r="U82" s="16">
-        <f t="shared" si="1"/>
         <v>46.150000000000006</v>
       </c>
       <c r="V82" s="15">
@@ -8460,7 +8127,6 @@
         <v>44.6</v>
       </c>
       <c r="X82" s="16">
-        <f t="shared" si="2"/>
         <v>51.45</v>
       </c>
       <c r="Y82" s="15">
@@ -8470,7 +8136,6 @@
         <v>49.7</v>
       </c>
       <c r="AA82" s="16">
-        <f t="shared" si="3"/>
         <v>-5.6</v>
       </c>
       <c r="AB82" s="15">
@@ -8503,7 +8168,6 @@
         <v>44636</v>
       </c>
       <c r="H83" s="14">
-        <f t="shared" si="0"/>
         <v>69</v>
       </c>
       <c r="I83" s="15">
@@ -8543,7 +8207,6 @@
         <v>602</v>
       </c>
       <c r="U83" s="16">
-        <f t="shared" si="1"/>
         <v>42.400000000000006</v>
       </c>
       <c r="V83" s="15">
@@ -8553,7 +8216,6 @@
         <v>42.1</v>
       </c>
       <c r="X83" s="16">
-        <f t="shared" si="2"/>
         <v>47.2</v>
       </c>
       <c r="Y83" s="15">
@@ -8563,7 +8225,6 @@
         <v>46.9</v>
       </c>
       <c r="AA83" s="16">
-        <f t="shared" si="3"/>
         <v>-5.75</v>
       </c>
       <c r="AB83" s="15">
@@ -8596,7 +8257,6 @@
         <v>44629</v>
       </c>
       <c r="H84" s="14">
-        <f t="shared" si="0"/>
         <v>63</v>
       </c>
       <c r="I84" s="15">
@@ -8624,7 +8284,6 @@
         <v>5.56</v>
       </c>
       <c r="Q84" s="15">
-        <f>T84</f>
         <v>509</v>
       </c>
       <c r="R84" s="15">
@@ -8637,7 +8296,6 @@
         <v>509</v>
       </c>
       <c r="U84" s="16">
-        <f t="shared" si="1"/>
         <v>42.55</v>
       </c>
       <c r="V84" s="15">
@@ -8647,7 +8305,6 @@
         <v>41.7</v>
       </c>
       <c r="X84" s="16">
-        <f t="shared" si="2"/>
         <v>47.4</v>
       </c>
       <c r="Y84" s="15">
@@ -8657,7 +8314,6 @@
         <v>46.5</v>
       </c>
       <c r="AA84" s="16">
-        <f t="shared" si="3"/>
         <v>-5.55</v>
       </c>
       <c r="AB84" s="15">
@@ -8690,7 +8346,6 @@
         <v>44657</v>
       </c>
       <c r="H85" s="14">
-        <f t="shared" si="0"/>
         <v>57</v>
       </c>
       <c r="I85" s="15">
@@ -8730,7 +8385,6 @@
         <v>663</v>
       </c>
       <c r="U85" s="16">
-        <f t="shared" si="1"/>
         <v>42.05</v>
       </c>
       <c r="V85" s="15">
@@ -8740,7 +8394,6 @@
         <v>41.9</v>
       </c>
       <c r="X85" s="16">
-        <f t="shared" si="2"/>
         <v>46.900000000000006</v>
       </c>
       <c r="Y85" s="15">
@@ -8750,7 +8403,6 @@
         <v>46.7</v>
       </c>
       <c r="AA85" s="16">
-        <f t="shared" si="3"/>
         <v>-5.7</v>
       </c>
       <c r="AB85" s="15">
@@ -8783,7 +8435,6 @@
         <v>44902</v>
       </c>
       <c r="H86" s="14">
-        <f t="shared" si="0"/>
         <v>65</v>
       </c>
       <c r="I86" s="15">
@@ -8823,7 +8474,6 @@
         <v>580</v>
       </c>
       <c r="U86" s="16">
-        <f t="shared" si="1"/>
         <v>45.3</v>
       </c>
       <c r="V86" s="15">
@@ -8833,7 +8483,6 @@
         <v>45.2</v>
       </c>
       <c r="X86" s="16">
-        <f t="shared" si="2"/>
         <v>50.45</v>
       </c>
       <c r="Y86" s="15">
@@ -8843,7 +8492,6 @@
         <v>50.4</v>
       </c>
       <c r="AA86" s="16">
-        <f t="shared" si="3"/>
         <v>-5.85</v>
       </c>
       <c r="AB86" s="15">
@@ -8876,7 +8524,6 @@
         <v>44690</v>
       </c>
       <c r="H87" s="14">
-        <f t="shared" si="0"/>
         <v>71</v>
       </c>
       <c r="I87" s="15">
@@ -8904,7 +8551,6 @@
         <v>5.47</v>
       </c>
       <c r="Q87" s="15">
-        <f>T87</f>
         <v>705</v>
       </c>
       <c r="R87" s="15">
@@ -8917,7 +8563,6 @@
         <v>705</v>
       </c>
       <c r="U87" s="16">
-        <f t="shared" si="1"/>
         <v>40.200000000000003</v>
       </c>
       <c r="V87" s="15">
@@ -8927,7 +8572,6 @@
         <v>39.700000000000003</v>
       </c>
       <c r="X87" s="16">
-        <f t="shared" si="2"/>
         <v>44.8</v>
       </c>
       <c r="Y87" s="15">
@@ -8937,7 +8581,6 @@
         <v>44.3</v>
       </c>
       <c r="AA87" s="16">
-        <f t="shared" si="3"/>
         <v>-6.5</v>
       </c>
       <c r="AB87" s="15">
@@ -8970,7 +8613,6 @@
         <v>44595</v>
       </c>
       <c r="H88" s="14">
-        <f t="shared" si="0"/>
         <v>60</v>
       </c>
       <c r="I88" s="15">
@@ -9010,7 +8652,6 @@
         <v>511</v>
       </c>
       <c r="U88" s="16">
-        <f t="shared" si="1"/>
         <v>45.45</v>
       </c>
       <c r="V88" s="15">
@@ -9020,7 +8661,6 @@
         <v>45.2</v>
       </c>
       <c r="X88" s="16">
-        <f t="shared" si="2"/>
         <v>50.599999999999994</v>
       </c>
       <c r="Y88" s="15">
@@ -9030,7 +8670,6 @@
         <v>50.3</v>
       </c>
       <c r="AA88" s="16">
-        <f t="shared" si="3"/>
         <v>-6.35</v>
       </c>
       <c r="AB88" s="15">
@@ -9063,7 +8702,6 @@
         <v>44356</v>
       </c>
       <c r="H89" s="14">
-        <f t="shared" si="0"/>
         <v>76</v>
       </c>
       <c r="I89" s="15">
@@ -9103,7 +8741,6 @@
         <v>505</v>
       </c>
       <c r="U89" s="16">
-        <f t="shared" si="1"/>
         <v>45.25</v>
       </c>
       <c r="V89" s="15">
@@ -9113,7 +8750,6 @@
         <v>45.1</v>
       </c>
       <c r="X89" s="16">
-        <f t="shared" si="2"/>
         <v>50.45</v>
       </c>
       <c r="Y89" s="15">
@@ -9123,7 +8759,6 @@
         <v>50.3</v>
       </c>
       <c r="AA89" s="16">
-        <f t="shared" si="3"/>
         <v>-6.15</v>
       </c>
       <c r="AB89" s="15">
@@ -9156,7 +8791,6 @@
         <v>44454</v>
       </c>
       <c r="H90" s="14">
-        <f t="shared" si="0"/>
         <v>76</v>
       </c>
       <c r="I90" s="15">
@@ -9196,7 +8830,6 @@
         <v>509</v>
       </c>
       <c r="U90" s="16">
-        <f t="shared" si="1"/>
         <v>45.75</v>
       </c>
       <c r="V90" s="15">
@@ -9206,7 +8839,6 @@
         <v>45.4</v>
       </c>
       <c r="X90" s="16">
-        <f t="shared" si="2"/>
         <v>51</v>
       </c>
       <c r="Y90" s="15">
@@ -9216,7 +8848,6 @@
         <v>50.6</v>
       </c>
       <c r="AA90" s="16">
-        <f t="shared" si="3"/>
         <v>-6.25</v>
       </c>
       <c r="AB90" s="15">
@@ -9249,7 +8880,6 @@
         <v>43761</v>
       </c>
       <c r="H91" s="14">
-        <f t="shared" si="0"/>
         <v>62</v>
       </c>
       <c r="I91" s="15">
@@ -9289,7 +8919,6 @@
         <v>595</v>
       </c>
       <c r="U91" s="16">
-        <f t="shared" si="1"/>
         <v>43.15</v>
       </c>
       <c r="V91" s="15">
@@ -9299,7 +8928,6 @@
         <v>42.8</v>
       </c>
       <c r="X91" s="16">
-        <f t="shared" si="2"/>
         <v>48.05</v>
       </c>
       <c r="Y91" s="15">
@@ -9309,7 +8937,6 @@
         <v>47.7</v>
       </c>
       <c r="AA91" s="16">
-        <f t="shared" si="3"/>
         <v>-5.55</v>
       </c>
       <c r="AB91" s="15">
@@ -9342,7 +8969,6 @@
         <v>45371</v>
       </c>
       <c r="H92" s="14">
-        <f t="shared" si="0"/>
         <v>66</v>
       </c>
       <c r="I92" s="15">
@@ -9382,7 +9008,6 @@
         <v>561</v>
       </c>
       <c r="U92" s="16">
-        <f t="shared" si="1"/>
         <v>42.650000000000006</v>
       </c>
       <c r="V92" s="15">
@@ -9392,7 +9017,6 @@
         <v>42.2</v>
       </c>
       <c r="X92" s="16">
-        <f t="shared" si="2"/>
         <v>47.5</v>
       </c>
       <c r="Y92" s="15">
@@ -9402,7 +9026,6 @@
         <v>47</v>
       </c>
       <c r="AA92" s="16">
-        <f t="shared" si="3"/>
         <v>-5.75</v>
       </c>
       <c r="AB92" s="15">
@@ -9435,7 +9058,6 @@
         <v>44741</v>
       </c>
       <c r="H93" s="14">
-        <f t="shared" si="0"/>
         <v>68</v>
       </c>
       <c r="I93" s="15">
@@ -9475,7 +9097,6 @@
         <v>584</v>
       </c>
       <c r="U93" s="16">
-        <f t="shared" si="1"/>
         <v>44.9</v>
       </c>
       <c r="V93" s="15">
@@ -9485,7 +9106,6 @@
         <v>44.3</v>
       </c>
       <c r="X93" s="16">
-        <f t="shared" si="2"/>
         <v>50</v>
       </c>
       <c r="Y93" s="15">
@@ -9495,7 +9115,6 @@
         <v>49.3</v>
       </c>
       <c r="AA93" s="16">
-        <f t="shared" si="3"/>
         <v>-5.95</v>
       </c>
       <c r="AB93" s="15">
@@ -9528,7 +9147,6 @@
         <v>44741</v>
       </c>
       <c r="H94" s="14">
-        <f t="shared" si="0"/>
         <v>55</v>
       </c>
       <c r="I94" s="15">
@@ -9556,7 +9174,6 @@
         <v>4.78</v>
       </c>
       <c r="Q94" s="15">
-        <f>T94</f>
         <v>579</v>
       </c>
       <c r="R94" s="15">
@@ -9569,7 +9186,6 @@
         <v>579</v>
       </c>
       <c r="U94" s="16">
-        <f t="shared" si="1"/>
         <v>42.099999999999994</v>
       </c>
       <c r="V94" s="15">
@@ -9579,7 +9195,6 @@
         <v>41.9</v>
       </c>
       <c r="X94" s="16">
-        <f t="shared" si="2"/>
         <v>46.85</v>
       </c>
       <c r="Y94" s="15">
@@ -9589,7 +9204,6 @@
         <v>46.6</v>
       </c>
       <c r="AA94" s="16">
-        <f t="shared" si="3"/>
         <v>-5.55</v>
       </c>
       <c r="AB94" s="15">
@@ -9622,7 +9236,6 @@
         <v>44650</v>
       </c>
       <c r="H95" s="14">
-        <f t="shared" si="0"/>
         <v>54</v>
       </c>
       <c r="I95" s="15">
@@ -9662,7 +9275,6 @@
         <v>556</v>
       </c>
       <c r="U95" s="16">
-        <f t="shared" si="1"/>
         <v>42.5</v>
       </c>
       <c r="V95" s="15">
@@ -9672,7 +9284,6 @@
         <v>41.6</v>
       </c>
       <c r="X95" s="16">
-        <f t="shared" si="2"/>
         <v>47.3</v>
       </c>
       <c r="Y95" s="15">
@@ -9682,7 +9293,6 @@
         <v>46.3</v>
       </c>
       <c r="AA95" s="16">
-        <f t="shared" si="3"/>
         <v>-5.65</v>
       </c>
       <c r="AB95" s="15">
@@ -9715,7 +9325,6 @@
         <v>45238</v>
       </c>
       <c r="H96" s="14">
-        <f t="shared" si="0"/>
         <v>56</v>
       </c>
       <c r="I96" s="15">
@@ -9755,7 +9364,6 @@
         <v>558</v>
       </c>
       <c r="U96" s="16">
-        <f t="shared" si="1"/>
         <v>43.25</v>
       </c>
       <c r="V96" s="15">
@@ -9765,7 +9373,6 @@
         <v>42.2</v>
       </c>
       <c r="X96" s="16">
-        <f t="shared" si="2"/>
         <v>48.2</v>
       </c>
       <c r="Y96" s="15">
@@ -9775,7 +9382,6 @@
         <v>47.1</v>
       </c>
       <c r="AA96" s="16">
-        <f t="shared" si="3"/>
         <v>-5.7</v>
       </c>
       <c r="AB96" s="15">
@@ -9808,7 +9414,6 @@
         <v>44958</v>
       </c>
       <c r="H97" s="14">
-        <f t="shared" si="0"/>
         <v>62</v>
       </c>
       <c r="I97" s="15">
@@ -9848,7 +9453,6 @@
         <v>641</v>
       </c>
       <c r="U97" s="16">
-        <f t="shared" si="1"/>
         <v>45.95</v>
       </c>
       <c r="V97" s="15">
@@ -9858,7 +9462,6 @@
         <v>45</v>
       </c>
       <c r="X97" s="16">
-        <f t="shared" si="2"/>
         <v>51.2</v>
       </c>
       <c r="Y97" s="15">
@@ -9868,7 +9471,6 @@
         <v>50.1</v>
       </c>
       <c r="AA97" s="16">
-        <f t="shared" si="3"/>
         <v>-6.5</v>
       </c>
       <c r="AB97" s="15">
@@ -9901,7 +9503,6 @@
         <v>44895</v>
       </c>
       <c r="H98" s="14">
-        <f t="shared" si="0"/>
         <v>60</v>
       </c>
       <c r="I98" s="15">
@@ -9929,7 +9530,6 @@
         <v>4.2699999999999996</v>
       </c>
       <c r="Q98" s="15">
-        <f>T98</f>
         <v>880</v>
       </c>
       <c r="R98" s="15">
@@ -9942,7 +9542,6 @@
         <v>880</v>
       </c>
       <c r="U98" s="16">
-        <f t="shared" si="1"/>
         <v>47.1</v>
       </c>
       <c r="V98" s="15">
@@ -9952,7 +9551,6 @@
         <v>46.2</v>
       </c>
       <c r="X98" s="16">
-        <f t="shared" si="2"/>
         <v>52.45</v>
       </c>
       <c r="Y98" s="15">
@@ -9962,7 +9560,6 @@
         <v>51.5</v>
       </c>
       <c r="AA98" s="16">
-        <f t="shared" si="3"/>
         <v>-6.6</v>
       </c>
       <c r="AB98" s="15">

</xml_diff>

<commit_message>
Refactor code structure for improved readability and maintainability
</commit_message>
<xml_diff>
--- a/FacoDMEK.xlsx
+++ b/FacoDMEK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Websites\faco-dmek\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42182927-20E1-46DA-8645-BB9F42D57FBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC8A08A-EB15-4723-95B2-5DCED019C40D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -833,7 +833,7 @@
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="S44" sqref="S44"/>
+      <selection pane="bottomLeft" activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.2109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -992,7 +992,7 @@
         <v>12</v>
       </c>
       <c r="S2" s="15">
-        <v>115.3</v>
+        <v>118.4</v>
       </c>
       <c r="T2" s="15">
         <v>594</v>

</xml_diff>

<commit_message>
Update FacoDMEK.xlsx with revised data and remove temporary file
</commit_message>
<xml_diff>
--- a/FacoDMEK.xlsx
+++ b/FacoDMEK.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Websites\faco-dmek\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41A83018-24CF-4496-8462-A53252783259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDA82E95-06E9-4B14-B86C-2C9971C2A6C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cleaned Data" sheetId="2" r:id="rId1"/>
+    <sheet name="Foglio1" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Cleaned Data'!$B$1:$AC$98</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Cleaned Data'!$B$1:$AC$97</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -828,12 +829,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AC98"/>
+  <dimension ref="A1:AC97"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="J103" sqref="J103"/>
+      <selection pane="bottomLeft" activeCell="B98" sqref="A98:XFD98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.5"/>
@@ -9480,95 +9481,6 @@
         <v>-5.8</v>
       </c>
     </row>
-    <row r="98" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A98" s="9">
-        <v>97</v>
-      </c>
-      <c r="B98" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C98" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D98" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E98" s="13">
-        <v>21702</v>
-      </c>
-      <c r="F98" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G98" s="13">
-        <v>44755</v>
-      </c>
-      <c r="H98" s="14">
-        <v>63</v>
-      </c>
-      <c r="I98" s="15">
-        <v>0.6</v>
-      </c>
-      <c r="J98" s="16">
-        <v>5</v>
-      </c>
-      <c r="K98" s="15">
-        <v>27.48</v>
-      </c>
-      <c r="L98" s="15">
-        <v>41.2</v>
-      </c>
-      <c r="M98" s="15">
-        <v>39.4</v>
-      </c>
-      <c r="N98" s="15">
-        <v>2.8</v>
-      </c>
-      <c r="O98" s="15">
-        <v>11.19</v>
-      </c>
-      <c r="P98" s="15">
-        <v>4.9400000000000004</v>
-      </c>
-      <c r="Q98" s="15">
-        <v>403</v>
-      </c>
-      <c r="R98" s="15">
-        <v>16.5</v>
-      </c>
-      <c r="S98" s="15">
-        <v>118.5</v>
-      </c>
-      <c r="T98" s="15">
-        <v>448</v>
-      </c>
-      <c r="U98" s="16">
-        <v>40.299999999999997</v>
-      </c>
-      <c r="V98" s="15">
-        <v>41.2</v>
-      </c>
-      <c r="W98" s="15">
-        <v>39.4</v>
-      </c>
-      <c r="X98" s="16">
-        <v>44.9</v>
-      </c>
-      <c r="Y98" s="15">
-        <v>45.9</v>
-      </c>
-      <c r="Z98" s="15">
-        <v>43.9</v>
-      </c>
-      <c r="AA98" s="16">
-        <v>-6.25</v>
-      </c>
-      <c r="AB98" s="15">
-        <v>-6.4</v>
-      </c>
-      <c r="AC98" s="15">
-        <v>-6.1</v>
-      </c>
-    </row>
   </sheetData>
   <autoFilter ref="B1:AC98" xr:uid="{00000000-0009-0000-0000-000001000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:AC98">
@@ -9578,4 +9490,108 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52A34D5A-AE00-4127-BB91-B6A5C0A7592F}">
+  <dimension ref="A1:AC1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetData>
+    <row r="1" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="9">
+        <v>97</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="13">
+        <v>21702</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="G1" s="13">
+        <v>44755</v>
+      </c>
+      <c r="H1" s="14">
+        <v>63</v>
+      </c>
+      <c r="I1" s="15">
+        <v>0.6</v>
+      </c>
+      <c r="J1" s="16">
+        <v>5</v>
+      </c>
+      <c r="K1" s="15">
+        <v>27.48</v>
+      </c>
+      <c r="L1" s="15">
+        <v>41.2</v>
+      </c>
+      <c r="M1" s="15">
+        <v>39.4</v>
+      </c>
+      <c r="N1" s="15">
+        <v>2.8</v>
+      </c>
+      <c r="O1" s="15">
+        <v>11.19</v>
+      </c>
+      <c r="P1" s="15">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="Q1" s="15">
+        <v>403</v>
+      </c>
+      <c r="R1" s="15">
+        <v>16.5</v>
+      </c>
+      <c r="S1" s="15">
+        <v>118.5</v>
+      </c>
+      <c r="T1" s="15">
+        <v>448</v>
+      </c>
+      <c r="U1" s="16">
+        <v>40.299999999999997</v>
+      </c>
+      <c r="V1" s="15">
+        <v>41.2</v>
+      </c>
+      <c r="W1" s="15">
+        <v>39.4</v>
+      </c>
+      <c r="X1" s="16">
+        <v>44.9</v>
+      </c>
+      <c r="Y1" s="15">
+        <v>45.9</v>
+      </c>
+      <c r="Z1" s="15">
+        <v>43.9</v>
+      </c>
+      <c r="AA1" s="16">
+        <v>-6.25</v>
+      </c>
+      <c r="AB1" s="15">
+        <v>-6.4</v>
+      </c>
+      <c r="AC1" s="15">
+        <v>-6.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Implement code changes to enhance functionality and improve performance
</commit_message>
<xml_diff>
--- a/FacoDMEK.xlsx
+++ b/FacoDMEK.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Websites\faco-dmek\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDA82E95-06E9-4B14-B86C-2C9971C2A6C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE9EBDA8-40D2-4793-AA9C-9CE481C36323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Cleaned Data" sheetId="2" r:id="rId1"/>
-    <sheet name="Foglio1" sheetId="3" r:id="rId2"/>
+    <sheet name="Data" sheetId="2" r:id="rId1"/>
+    <sheet name="Excluded" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Cleaned Data'!$B$1:$AC$97</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$B$1:$AC$97</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="115">
   <si>
     <t>IOL Power</t>
   </si>
@@ -831,24 +831,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="B98" sqref="A98:XFD98"/>
+      <selection pane="bottomLeft" activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="11.2109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="19.4375" customWidth="1"/>
-    <col min="3" max="8" width="10.1875" customWidth="1"/>
-    <col min="9" max="10" width="14.875" customWidth="1"/>
-    <col min="11" max="18" width="10.1875" customWidth="1"/>
-    <col min="19" max="19" width="13.6875" customWidth="1"/>
-    <col min="20" max="29" width="10.1875" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="3" max="8" width="10.2109375" customWidth="1"/>
+    <col min="9" max="10" width="14.85546875" customWidth="1"/>
+    <col min="11" max="18" width="10.2109375" customWidth="1"/>
+    <col min="19" max="19" width="13.7109375" customWidth="1"/>
+    <col min="20" max="29" width="10.2109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="52.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:29" ht="52.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>87</v>
       </c>
@@ -937,7 +937,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="9">
         <v>1</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>-4.0999999999999996</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="9">
         <v>2</v>
       </c>
@@ -1115,7 +1115,7 @@
         <v>-6.4</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="9">
         <v>3</v>
       </c>
@@ -1204,7 +1204,7 @@
         <v>-6.2</v>
       </c>
     </row>
-    <row r="5" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="9">
         <v>4</v>
       </c>
@@ -1293,7 +1293,7 @@
         <v>-5.9</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="9">
         <v>5</v>
       </c>
@@ -1382,7 +1382,7 @@
         <v>-5.3</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="9">
         <v>6</v>
       </c>
@@ -1471,7 +1471,7 @@
         <v>-6.3</v>
       </c>
     </row>
-    <row r="8" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="9">
         <v>7</v>
       </c>
@@ -1560,7 +1560,7 @@
         <v>-5.7</v>
       </c>
     </row>
-    <row r="9" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="9">
         <v>8</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>-5.3</v>
       </c>
     </row>
-    <row r="10" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="9">
         <v>9</v>
       </c>
@@ -1738,7 +1738,7 @@
         <v>-5.3</v>
       </c>
     </row>
-    <row r="11" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="9">
         <v>10</v>
       </c>
@@ -1827,7 +1827,7 @@
         <v>-6.1</v>
       </c>
     </row>
-    <row r="12" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="9">
         <v>11</v>
       </c>
@@ -1916,7 +1916,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="13" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="9">
         <v>12</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>-5.7</v>
       </c>
     </row>
-    <row r="14" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="9">
         <v>13</v>
       </c>
@@ -2094,7 +2094,7 @@
         <v>-6.2</v>
       </c>
     </row>
-    <row r="15" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="9">
         <v>14</v>
       </c>
@@ -2183,7 +2183,7 @@
         <v>-5.4</v>
       </c>
     </row>
-    <row r="16" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="9">
         <v>15</v>
       </c>
@@ -2272,7 +2272,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="17" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="9">
         <v>16</v>
       </c>
@@ -2361,7 +2361,7 @@
         <v>-6.1</v>
       </c>
     </row>
-    <row r="18" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="9">
         <v>17</v>
       </c>
@@ -2450,7 +2450,7 @@
         <v>-6.2</v>
       </c>
     </row>
-    <row r="19" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="9">
         <v>18</v>
       </c>
@@ -2539,7 +2539,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="20" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="9">
         <v>19</v>
       </c>
@@ -2628,7 +2628,7 @@
         <v>-5.8</v>
       </c>
     </row>
-    <row r="21" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="9">
         <v>20</v>
       </c>
@@ -2717,7 +2717,7 @@
         <v>-5.5</v>
       </c>
     </row>
-    <row r="22" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="9">
         <v>21</v>
       </c>
@@ -2806,7 +2806,7 @@
         <v>-5.6</v>
       </c>
     </row>
-    <row r="23" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="9">
         <v>22</v>
       </c>
@@ -2895,7 +2895,7 @@
         <v>-5.3</v>
       </c>
     </row>
-    <row r="24" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="9">
         <v>23</v>
       </c>
@@ -2984,7 +2984,7 @@
         <v>-6.4</v>
       </c>
     </row>
-    <row r="25" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="9">
         <v>24</v>
       </c>
@@ -3073,7 +3073,7 @@
         <v>-5.2</v>
       </c>
     </row>
-    <row r="26" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="9">
         <v>25</v>
       </c>
@@ -3162,7 +3162,7 @@
         <v>-5.4</v>
       </c>
     </row>
-    <row r="27" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="9">
         <v>26</v>
       </c>
@@ -3251,7 +3251,7 @@
         <v>-5.5</v>
       </c>
     </row>
-    <row r="28" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="9">
         <v>27</v>
       </c>
@@ -3340,7 +3340,7 @@
         <v>-6.2</v>
       </c>
     </row>
-    <row r="29" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="9">
         <v>28</v>
       </c>
@@ -3429,7 +3429,7 @@
         <v>-5.3</v>
       </c>
     </row>
-    <row r="30" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="9">
         <v>29</v>
       </c>
@@ -3518,7 +3518,7 @@
         <v>-5.5</v>
       </c>
     </row>
-    <row r="31" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="9">
         <v>30</v>
       </c>
@@ -3607,7 +3607,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="32" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="9">
         <v>31</v>
       </c>
@@ -3696,7 +3696,7 @@
         <v>-5.6</v>
       </c>
     </row>
-    <row r="33" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="9">
         <v>32</v>
       </c>
@@ -3785,7 +3785,7 @@
         <v>-5.5</v>
       </c>
     </row>
-    <row r="34" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="9">
         <v>33</v>
       </c>
@@ -3874,7 +3874,7 @@
         <v>-5.2</v>
       </c>
     </row>
-    <row r="35" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="9">
         <v>34</v>
       </c>
@@ -3963,7 +3963,7 @@
         <v>-5.9</v>
       </c>
     </row>
-    <row r="36" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="9">
         <v>35</v>
       </c>
@@ -4052,7 +4052,7 @@
         <v>-5.2</v>
       </c>
     </row>
-    <row r="37" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="9">
         <v>36</v>
       </c>
@@ -4141,7 +4141,7 @@
         <v>-5.7</v>
       </c>
     </row>
-    <row r="38" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="9">
         <v>37</v>
       </c>
@@ -4230,7 +4230,7 @@
         <v>-5.4</v>
       </c>
     </row>
-    <row r="39" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="9">
         <v>38</v>
       </c>
@@ -4319,7 +4319,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="40" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="9">
         <v>39</v>
       </c>
@@ -4408,7 +4408,7 @@
         <v>-5.4</v>
       </c>
     </row>
-    <row r="41" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="9">
         <v>40</v>
       </c>
@@ -4497,7 +4497,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="42" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="9">
         <v>41</v>
       </c>
@@ -4586,7 +4586,7 @@
         <v>-5.5</v>
       </c>
     </row>
-    <row r="43" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="9">
         <v>42</v>
       </c>
@@ -4675,7 +4675,7 @@
         <v>-5.5</v>
       </c>
     </row>
-    <row r="44" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="9">
         <v>43</v>
       </c>
@@ -4764,7 +4764,7 @@
         <v>-5.3</v>
       </c>
     </row>
-    <row r="45" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="9">
         <v>44</v>
       </c>
@@ -4853,7 +4853,7 @@
         <v>-5.5</v>
       </c>
     </row>
-    <row r="46" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="9">
         <v>45</v>
       </c>
@@ -4942,7 +4942,7 @@
         <v>-5.5</v>
       </c>
     </row>
-    <row r="47" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="9">
         <v>46</v>
       </c>
@@ -5031,7 +5031,7 @@
         <v>-5.7</v>
       </c>
     </row>
-    <row r="48" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48" s="9">
         <v>47</v>
       </c>
@@ -5120,7 +5120,7 @@
         <v>-5.8</v>
       </c>
     </row>
-    <row r="49" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A49" s="9">
         <v>48</v>
       </c>
@@ -5209,7 +5209,7 @@
         <v>-4.5999999999999996</v>
       </c>
     </row>
-    <row r="50" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A50" s="9">
         <v>49</v>
       </c>
@@ -5298,7 +5298,7 @@
         <v>-5.7</v>
       </c>
     </row>
-    <row r="51" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A51" s="9">
         <v>50</v>
       </c>
@@ -5387,7 +5387,7 @@
         <v>-5.8</v>
       </c>
     </row>
-    <row r="52" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A52" s="9">
         <v>51</v>
       </c>
@@ -5476,7 +5476,7 @@
         <v>-5.9</v>
       </c>
     </row>
-    <row r="53" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A53" s="9">
         <v>52</v>
       </c>
@@ -5565,7 +5565,7 @@
         <v>-5.4</v>
       </c>
     </row>
-    <row r="54" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A54" s="9">
         <v>53</v>
       </c>
@@ -5654,7 +5654,7 @@
         <v>-5.2</v>
       </c>
     </row>
-    <row r="55" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A55" s="9">
         <v>54</v>
       </c>
@@ -5743,7 +5743,7 @@
         <v>-6.1</v>
       </c>
     </row>
-    <row r="56" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A56" s="9">
         <v>55</v>
       </c>
@@ -5832,7 +5832,7 @@
         <v>-5.7</v>
       </c>
     </row>
-    <row r="57" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A57" s="9">
         <v>56</v>
       </c>
@@ -5921,7 +5921,7 @@
         <v>-5.3</v>
       </c>
     </row>
-    <row r="58" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A58" s="9">
         <v>57</v>
       </c>
@@ -6010,7 +6010,7 @@
         <v>-5.8</v>
       </c>
     </row>
-    <row r="59" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A59" s="9">
         <v>58</v>
       </c>
@@ -6099,7 +6099,7 @@
         <v>-6.3</v>
       </c>
     </row>
-    <row r="60" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A60" s="9">
         <v>59</v>
       </c>
@@ -6188,7 +6188,7 @@
         <v>-5.3</v>
       </c>
     </row>
-    <row r="61" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A61" s="9">
         <v>60</v>
       </c>
@@ -6277,7 +6277,7 @@
         <v>-5.9</v>
       </c>
     </row>
-    <row r="62" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A62" s="9">
         <v>61</v>
       </c>
@@ -6366,7 +6366,7 @@
         <v>-5.9</v>
       </c>
     </row>
-    <row r="63" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A63" s="9">
         <v>62</v>
       </c>
@@ -6455,7 +6455,7 @@
         <v>-5.0999999999999996</v>
       </c>
     </row>
-    <row r="64" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="64" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A64" s="9">
         <v>63</v>
       </c>
@@ -6544,7 +6544,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="65" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A65" s="9">
         <v>64</v>
       </c>
@@ -6633,7 +6633,7 @@
         <v>-5.2</v>
       </c>
     </row>
-    <row r="66" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A66" s="9">
         <v>65</v>
       </c>
@@ -6722,7 +6722,7 @@
         <v>-6.3</v>
       </c>
     </row>
-    <row r="67" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A67" s="9">
         <v>66</v>
       </c>
@@ -6811,7 +6811,7 @@
         <v>-6.2</v>
       </c>
     </row>
-    <row r="68" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A68" s="9">
         <v>67</v>
       </c>
@@ -6900,7 +6900,7 @@
         <v>-5.7</v>
       </c>
     </row>
-    <row r="69" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A69" s="9">
         <v>68</v>
       </c>
@@ -6989,7 +6989,7 @@
         <v>-5.4</v>
       </c>
     </row>
-    <row r="70" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A70" s="9">
         <v>69</v>
       </c>
@@ -7078,7 +7078,7 @@
         <v>-5.5</v>
       </c>
     </row>
-    <row r="71" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A71" s="9">
         <v>70</v>
       </c>
@@ -7167,7 +7167,7 @@
         <v>-5.7</v>
       </c>
     </row>
-    <row r="72" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A72" s="9">
         <v>71</v>
       </c>
@@ -7256,7 +7256,7 @@
         <v>-5.8</v>
       </c>
     </row>
-    <row r="73" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A73" s="9">
         <v>72</v>
       </c>
@@ -7345,7 +7345,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="74" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A74" s="9">
         <v>73</v>
       </c>
@@ -7434,7 +7434,7 @@
         <v>-6.3</v>
       </c>
     </row>
-    <row r="75" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A75" s="9">
         <v>74</v>
       </c>
@@ -7523,7 +7523,7 @@
         <v>-5.2</v>
       </c>
     </row>
-    <row r="76" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A76" s="9">
         <v>75</v>
       </c>
@@ -7612,7 +7612,7 @@
         <v>-5.3</v>
       </c>
     </row>
-    <row r="77" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A77" s="9">
         <v>76</v>
       </c>
@@ -7701,7 +7701,7 @@
         <v>-5.2</v>
       </c>
     </row>
-    <row r="78" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A78" s="9">
         <v>77</v>
       </c>
@@ -7790,7 +7790,7 @@
         <v>-5.5</v>
       </c>
     </row>
-    <row r="79" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A79" s="9">
         <v>78</v>
       </c>
@@ -7879,7 +7879,7 @@
         <v>-5.3</v>
       </c>
     </row>
-    <row r="80" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="80" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A80" s="9">
         <v>79</v>
       </c>
@@ -7968,7 +7968,7 @@
         <v>-5.7</v>
       </c>
     </row>
-    <row r="81" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="81" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A81" s="9">
         <v>80</v>
       </c>
@@ -8057,7 +8057,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="82" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="82" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A82" s="9">
         <v>81</v>
       </c>
@@ -8146,7 +8146,7 @@
         <v>-5.0999999999999996</v>
       </c>
     </row>
-    <row r="83" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="83" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A83" s="9">
         <v>82</v>
       </c>
@@ -8235,7 +8235,7 @@
         <v>-5.7</v>
       </c>
     </row>
-    <row r="84" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="84" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A84" s="9">
         <v>83</v>
       </c>
@@ -8324,7 +8324,7 @@
         <v>-5.0999999999999996</v>
       </c>
     </row>
-    <row r="85" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="85" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A85" s="9">
         <v>84</v>
       </c>
@@ -8413,7 +8413,7 @@
         <v>-5.5</v>
       </c>
     </row>
-    <row r="86" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="86" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A86" s="9">
         <v>85</v>
       </c>
@@ -8502,7 +8502,7 @@
         <v>-5.6</v>
       </c>
     </row>
-    <row r="87" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="87" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A87" s="9">
         <v>86</v>
       </c>
@@ -8591,7 +8591,7 @@
         <v>-5.8</v>
       </c>
     </row>
-    <row r="88" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="88" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A88" s="9">
         <v>87</v>
       </c>
@@ -8680,7 +8680,7 @@
         <v>-5.0999999999999996</v>
       </c>
     </row>
-    <row r="89" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="89" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A89" s="9">
         <v>88</v>
       </c>
@@ -8769,7 +8769,7 @@
         <v>-5.9</v>
       </c>
     </row>
-    <row r="90" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="90" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A90" s="9">
         <v>89</v>
       </c>
@@ -8858,7 +8858,7 @@
         <v>-5.7</v>
       </c>
     </row>
-    <row r="91" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="91" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A91" s="9">
         <v>90</v>
       </c>
@@ -8947,7 +8947,7 @@
         <v>-6.1</v>
       </c>
     </row>
-    <row r="92" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="92" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A92" s="9">
         <v>91</v>
       </c>
@@ -9036,7 +9036,7 @@
         <v>-5.9</v>
       </c>
     </row>
-    <row r="93" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="93" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A93" s="9">
         <v>92</v>
       </c>
@@ -9125,7 +9125,7 @@
         <v>-5.5</v>
       </c>
     </row>
-    <row r="94" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="94" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A94" s="9">
         <v>93</v>
       </c>
@@ -9214,7 +9214,7 @@
         <v>-5.6</v>
       </c>
     </row>
-    <row r="95" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="95" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A95" s="9">
         <v>94</v>
       </c>
@@ -9303,7 +9303,7 @@
         <v>-5.5</v>
       </c>
     </row>
-    <row r="96" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="96" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A96" s="9">
         <v>95</v>
       </c>
@@ -9392,7 +9392,7 @@
         <v>-5.6</v>
       </c>
     </row>
-    <row r="97" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="97" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A97" s="9">
         <v>96</v>
       </c>
@@ -9494,100 +9494,189 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52A34D5A-AE00-4127-BB91-B6A5C0A7592F}">
-  <dimension ref="A1:AC1"/>
+  <dimension ref="A1:AC2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="9">
+    <row r="1" spans="1:29" ht="52.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L1" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="M1" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="X1" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="Y1" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z1" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="AA1" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="AB1" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC1" s="8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="9">
+        <v>97</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="13">
+      <c r="E2" s="13">
         <v>21702</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F2" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="G1" s="13">
+      <c r="G2" s="13">
         <v>44755</v>
       </c>
-      <c r="H1" s="14">
+      <c r="H2" s="14">
         <v>63</v>
       </c>
-      <c r="I1" s="15">
+      <c r="I2" s="15">
         <v>0.6</v>
       </c>
-      <c r="J1" s="16">
+      <c r="J2" s="16">
         <v>5</v>
       </c>
-      <c r="K1" s="15">
+      <c r="K2" s="15">
         <v>27.48</v>
       </c>
-      <c r="L1" s="15">
+      <c r="L2" s="15">
         <v>41.2</v>
       </c>
-      <c r="M1" s="15">
+      <c r="M2" s="15">
         <v>39.4</v>
       </c>
-      <c r="N1" s="15">
+      <c r="N2" s="15">
         <v>2.8</v>
       </c>
-      <c r="O1" s="15">
+      <c r="O2" s="15">
         <v>11.19</v>
       </c>
-      <c r="P1" s="15">
+      <c r="P2" s="15">
         <v>4.9400000000000004</v>
       </c>
-      <c r="Q1" s="15">
+      <c r="Q2" s="15">
         <v>403</v>
       </c>
-      <c r="R1" s="15">
+      <c r="R2" s="15">
         <v>16.5</v>
       </c>
-      <c r="S1" s="15">
+      <c r="S2" s="15">
         <v>118.5</v>
       </c>
-      <c r="T1" s="15">
+      <c r="T2" s="15">
         <v>448</v>
       </c>
-      <c r="U1" s="16">
+      <c r="U2" s="16">
         <v>40.299999999999997</v>
       </c>
-      <c r="V1" s="15">
+      <c r="V2" s="15">
         <v>41.2</v>
       </c>
-      <c r="W1" s="15">
+      <c r="W2" s="15">
         <v>39.4</v>
       </c>
-      <c r="X1" s="16">
+      <c r="X2" s="16">
         <v>44.9</v>
       </c>
-      <c r="Y1" s="15">
+      <c r="Y2" s="15">
         <v>45.9</v>
       </c>
-      <c r="Z1" s="15">
+      <c r="Z2" s="15">
         <v>43.9</v>
       </c>
-      <c r="AA1" s="16">
+      <c r="AA2" s="16">
         <v>-6.25</v>
       </c>
-      <c r="AB1" s="15">
+      <c r="AB2" s="15">
         <v>-6.4</v>
       </c>
-      <c r="AC1" s="15">
+      <c r="AC2" s="15">
         <v>-6.1</v>
       </c>
     </row>

</xml_diff>